<commit_message>
ISP20220836 - Inspection2.0 功能調整
</commit_message>
<xml_diff>
--- a/Quality/Quality/XLT/InspBySPQuery_Detail.xlsx
+++ b/Quality/Quality/XLT/InspBySPQuery_Detail.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
   <si>
     <t>TOTAL</t>
   </si>
@@ -705,6 +705,10 @@
   </si>
   <si>
     <t>:</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>HT</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
 </sst>
@@ -712,9 +716,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.0"/>
-  </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -818,7 +819,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="59">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -1389,19 +1390,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1524,7 +1512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="229">
+  <cellXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1625,9 +1613,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1793,15 +1778,15 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1810,9 +1795,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1841,25 +1823,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1874,12 +1853,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1988,6 +1991,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2060,12 +2075,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2093,10 +2102,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2176,35 +2191,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2774,7 +2765,7 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:H5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2798,42 +2789,42 @@
     <row r="1" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:20" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="155"/>
-      <c r="D4" s="156"/>
-      <c r="E4" s="156"/>
-      <c r="F4" s="156"/>
-      <c r="G4" s="156"/>
-      <c r="H4" s="157"/>
-      <c r="I4" s="161" t="s">
+      <c r="C4" s="164"/>
+      <c r="D4" s="165"/>
+      <c r="E4" s="165"/>
+      <c r="F4" s="165"/>
+      <c r="G4" s="165"/>
+      <c r="H4" s="166"/>
+      <c r="I4" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="162"/>
-      <c r="K4" s="162"/>
-      <c r="L4" s="162"/>
-      <c r="M4" s="162"/>
-      <c r="N4" s="162"/>
-      <c r="O4" s="162"/>
-      <c r="P4" s="162"/>
-      <c r="Q4" s="162"/>
-      <c r="R4" s="163"/>
+      <c r="J4" s="171"/>
+      <c r="K4" s="171"/>
+      <c r="L4" s="171"/>
+      <c r="M4" s="171"/>
+      <c r="N4" s="171"/>
+      <c r="O4" s="171"/>
+      <c r="P4" s="171"/>
+      <c r="Q4" s="171"/>
+      <c r="R4" s="172"/>
     </row>
     <row r="5" spans="1:20" ht="10.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="158"/>
-      <c r="D5" s="159"/>
-      <c r="E5" s="159"/>
-      <c r="F5" s="159"/>
-      <c r="G5" s="159"/>
-      <c r="H5" s="160"/>
-      <c r="I5" s="164"/>
-      <c r="J5" s="165"/>
-      <c r="K5" s="165"/>
-      <c r="L5" s="165"/>
-      <c r="M5" s="165"/>
-      <c r="N5" s="165"/>
-      <c r="O5" s="165"/>
-      <c r="P5" s="165"/>
-      <c r="Q5" s="165"/>
-      <c r="R5" s="166"/>
+      <c r="C5" s="167"/>
+      <c r="D5" s="168"/>
+      <c r="E5" s="168"/>
+      <c r="F5" s="168"/>
+      <c r="G5" s="168"/>
+      <c r="H5" s="169"/>
+      <c r="I5" s="173"/>
+      <c r="J5" s="174"/>
+      <c r="K5" s="174"/>
+      <c r="L5" s="174"/>
+      <c r="M5" s="174"/>
+      <c r="N5" s="174"/>
+      <c r="O5" s="174"/>
+      <c r="P5" s="174"/>
+      <c r="Q5" s="174"/>
+      <c r="R5" s="175"/>
     </row>
     <row r="6" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="7" t="s">
@@ -2843,25 +2834,25 @@
       <c r="E6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="116"/>
+      <c r="F6" s="113"/>
       <c r="G6" s="17"/>
       <c r="H6" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="93"/>
-      <c r="J6" s="119" t="s">
+      <c r="I6" s="92"/>
+      <c r="J6" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="120"/>
-      <c r="L6" s="121"/>
+      <c r="K6" s="125"/>
+      <c r="L6" s="126"/>
       <c r="M6" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="N6" s="179"/>
-      <c r="O6" s="179"/>
-      <c r="P6" s="179"/>
-      <c r="Q6" s="179"/>
-      <c r="R6" s="180"/>
+      <c r="N6" s="114"/>
+      <c r="O6" s="114"/>
+      <c r="P6" s="114"/>
+      <c r="Q6" s="114"/>
+      <c r="R6" s="115"/>
       <c r="S6" s="20"/>
     </row>
     <row r="7" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2872,13 +2863,13 @@
       <c r="E7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="117"/>
-      <c r="G7" s="118"/>
-      <c r="H7" s="118"/>
-      <c r="I7" s="118"/>
-      <c r="J7" s="118"/>
-      <c r="K7" s="118"/>
-      <c r="L7" s="118"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="122"/>
+      <c r="I7" s="122"/>
+      <c r="J7" s="122"/>
+      <c r="K7" s="122"/>
+      <c r="L7" s="122"/>
       <c r="M7" s="11"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -2897,19 +2888,19 @@
       <c r="E8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="187"/>
-      <c r="G8" s="188"/>
-      <c r="H8" s="188"/>
-      <c r="I8" s="188"/>
-      <c r="J8" s="188"/>
-      <c r="K8" s="188"/>
-      <c r="L8" s="188"/>
-      <c r="M8" s="188"/>
-      <c r="N8" s="188"/>
-      <c r="O8" s="188"/>
-      <c r="P8" s="188"/>
-      <c r="Q8" s="188"/>
-      <c r="R8" s="189"/>
+      <c r="F8" s="194"/>
+      <c r="G8" s="195"/>
+      <c r="H8" s="195"/>
+      <c r="I8" s="195"/>
+      <c r="J8" s="195"/>
+      <c r="K8" s="195"/>
+      <c r="L8" s="195"/>
+      <c r="M8" s="195"/>
+      <c r="N8" s="195"/>
+      <c r="O8" s="195"/>
+      <c r="P8" s="195"/>
+      <c r="Q8" s="195"/>
+      <c r="R8" s="196"/>
       <c r="S8" s="20"/>
     </row>
     <row r="9" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2920,23 +2911,23 @@
       <c r="E9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="117"/>
-      <c r="G9" s="118"/>
-      <c r="H9" s="118"/>
-      <c r="I9" s="118"/>
-      <c r="J9" s="118"/>
-      <c r="K9" s="118"/>
-      <c r="L9" s="118"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="122"/>
+      <c r="H9" s="122"/>
+      <c r="I9" s="122"/>
+      <c r="J9" s="122"/>
+      <c r="K9" s="122"/>
+      <c r="L9" s="122"/>
       <c r="M9" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="N9" s="117"/>
-      <c r="O9" s="227"/>
-      <c r="P9" s="227"/>
-      <c r="Q9" s="227"/>
-      <c r="R9" s="228"/>
-      <c r="S9" s="115"/>
-      <c r="T9" s="226"/>
+      <c r="N9" s="123"/>
+      <c r="O9" s="197"/>
+      <c r="P9" s="197"/>
+      <c r="Q9" s="197"/>
+      <c r="R9" s="198"/>
+      <c r="S9" s="112"/>
+      <c r="T9" s="116"/>
     </row>
     <row r="10" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="8" t="s">
@@ -2946,13 +2937,13 @@
       <c r="E10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="117"/>
-      <c r="G10" s="118"/>
-      <c r="H10" s="118"/>
-      <c r="I10" s="118"/>
-      <c r="J10" s="118"/>
-      <c r="K10" s="118"/>
-      <c r="L10" s="118"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="122"/>
+      <c r="I10" s="122"/>
+      <c r="J10" s="122"/>
+      <c r="K10" s="122"/>
+      <c r="L10" s="122"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -2969,23 +2960,23 @@
       <c r="E11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="117"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="118"/>
-      <c r="J11" s="118"/>
-      <c r="K11" s="118"/>
-      <c r="L11" s="118"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="122"/>
+      <c r="H11" s="122"/>
+      <c r="I11" s="122"/>
+      <c r="J11" s="122"/>
+      <c r="K11" s="122"/>
+      <c r="L11" s="122"/>
       <c r="M11" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="N11" s="117"/>
-      <c r="O11" s="227"/>
-      <c r="P11" s="227"/>
-      <c r="Q11" s="227"/>
-      <c r="R11" s="228"/>
-      <c r="S11" s="115"/>
-      <c r="T11" s="115"/>
+      <c r="N11" s="123"/>
+      <c r="O11" s="197"/>
+      <c r="P11" s="197"/>
+      <c r="Q11" s="197"/>
+      <c r="R11" s="198"/>
+      <c r="S11" s="112"/>
+      <c r="T11" s="112"/>
     </row>
     <row r="12" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="8" t="s">
@@ -2995,13 +2986,13 @@
       <c r="E12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="117"/>
-      <c r="G12" s="118"/>
-      <c r="H12" s="118"/>
-      <c r="I12" s="118"/>
-      <c r="J12" s="118"/>
-      <c r="K12" s="118"/>
-      <c r="L12" s="118"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="122"/>
+      <c r="H12" s="122"/>
+      <c r="I12" s="122"/>
+      <c r="J12" s="122"/>
+      <c r="K12" s="122"/>
+      <c r="L12" s="122"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -3011,20 +3002,20 @@
       <c r="S12" s="20"/>
     </row>
     <row r="13" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="47" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="30"/>
       <c r="E13" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="117"/>
-      <c r="G13" s="118"/>
-      <c r="H13" s="118"/>
-      <c r="I13" s="118"/>
-      <c r="J13" s="118"/>
-      <c r="K13" s="118"/>
-      <c r="L13" s="118"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="122"/>
+      <c r="I13" s="122"/>
+      <c r="J13" s="122"/>
+      <c r="K13" s="122"/>
+      <c r="L13" s="122"/>
       <c r="M13" s="25"/>
       <c r="N13" s="25"/>
       <c r="O13" s="25"/>
@@ -3038,18 +3029,18 @@
         <v>30</v>
       </c>
       <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="64" t="s">
+      <c r="E14" s="117"/>
+      <c r="F14" s="118"/>
+      <c r="G14" s="118"/>
+      <c r="H14" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65" t="s">
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="L14" s="35" t="s">
+      <c r="L14" s="34" t="s">
         <v>28</v>
       </c>
       <c r="M14" s="33"/>
@@ -3057,47 +3048,47 @@
       <c r="O14" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="P14" s="35" t="s">
+      <c r="P14" s="34" t="s">
         <v>12</v>
       </c>
       <c r="Q14" s="33"/>
-      <c r="R14" s="36"/>
+      <c r="R14" s="35"/>
       <c r="S14" s="21"/>
     </row>
     <row r="15" spans="1:20" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="36" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="39" t="s">
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38" t="s">
         <v>40</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="40" t="s">
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="39" t="s">
         <v>32</v>
       </c>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="41"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="40"/>
       <c r="S15" s="20"/>
     </row>
     <row r="16" spans="1:20" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="41" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="27"/>
       <c r="E16" s="27"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="44"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="43"/>
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
       <c r="K16" s="27"/>
@@ -3107,32 +3098,32 @@
       <c r="O16" s="27"/>
       <c r="P16" s="27"/>
       <c r="Q16" s="27"/>
-      <c r="R16" s="45"/>
+      <c r="R16" s="44"/>
       <c r="S16" s="20"/>
     </row>
     <row r="17" spans="2:19" s="16" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="169" t="s">
+      <c r="C17" s="178" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="119"/>
-      <c r="E17" s="119"/>
-      <c r="F17" s="170"/>
-      <c r="G17" s="171" t="s">
+      <c r="D17" s="124"/>
+      <c r="E17" s="124"/>
+      <c r="F17" s="179"/>
+      <c r="G17" s="180" t="s">
         <v>77</v>
       </c>
-      <c r="H17" s="172"/>
-      <c r="I17" s="172"/>
-      <c r="J17" s="172"/>
-      <c r="K17" s="172"/>
-      <c r="L17" s="172"/>
-      <c r="M17" s="172"/>
-      <c r="N17" s="172"/>
-      <c r="O17" s="173" t="s">
+      <c r="H17" s="181"/>
+      <c r="I17" s="181"/>
+      <c r="J17" s="181"/>
+      <c r="K17" s="181"/>
+      <c r="L17" s="181"/>
+      <c r="M17" s="181"/>
+      <c r="N17" s="181"/>
+      <c r="O17" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="P17" s="174"/>
-      <c r="Q17" s="174"/>
-      <c r="R17" s="175"/>
+      <c r="P17" s="183"/>
+      <c r="Q17" s="183"/>
+      <c r="R17" s="184"/>
       <c r="S17" s="22"/>
     </row>
     <row r="18" spans="2:19" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3141,25 +3132,25 @@
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="95"/>
+      <c r="F18" s="94"/>
       <c r="G18" s="15" t="s">
         <v>19</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="95"/>
+      <c r="J18" s="94"/>
       <c r="K18" s="14" t="s">
         <v>17</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="95"/>
+      <c r="N18" s="94"/>
       <c r="O18" s="14" t="s">
         <v>37</v>
       </c>
       <c r="P18" s="12"/>
       <c r="Q18" s="12"/>
-      <c r="R18" s="106"/>
+      <c r="R18" s="104"/>
       <c r="S18" s="20"/>
     </row>
     <row r="19" spans="2:19" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3168,7 +3159,7 @@
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="95"/>
+      <c r="F19" s="94"/>
       <c r="G19" s="15" t="s">
         <v>20</v>
       </c>
@@ -3176,19 +3167,19 @@
       <c r="I19" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="J19" s="95"/>
+      <c r="J19" s="94"/>
       <c r="K19" s="14" t="s">
         <v>33</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="95"/>
-      <c r="O19" s="181" t="s">
+      <c r="N19" s="94"/>
+      <c r="O19" s="188" t="s">
         <v>74</v>
       </c>
-      <c r="P19" s="182"/>
-      <c r="Q19" s="183"/>
-      <c r="R19" s="106"/>
+      <c r="P19" s="189"/>
+      <c r="Q19" s="190"/>
+      <c r="R19" s="104"/>
       <c r="S19" s="20"/>
     </row>
     <row r="20" spans="2:19" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3197,13 +3188,13 @@
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="95"/>
+      <c r="F20" s="94"/>
       <c r="G20" s="15" t="s">
         <v>21</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="95"/>
+      <c r="J20" s="94"/>
       <c r="K20" s="14" t="s">
         <v>34</v>
       </c>
@@ -3211,704 +3202,699 @@
       <c r="M20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N20" s="95"/>
-      <c r="O20" s="184" t="s">
+      <c r="N20" s="94"/>
+      <c r="O20" s="191" t="s">
         <v>36</v>
       </c>
-      <c r="P20" s="185"/>
-      <c r="Q20" s="186"/>
-      <c r="R20" s="106"/>
-      <c r="S20" s="105"/>
+      <c r="P20" s="192"/>
+      <c r="Q20" s="193"/>
+      <c r="R20" s="104"/>
+      <c r="S20" s="103"/>
     </row>
     <row r="21" spans="2:19" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
+      <c r="C21" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="49"/>
       <c r="E21" s="25"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="50" t="s">
+      <c r="F21" s="94"/>
+      <c r="G21" s="49" t="s">
         <v>22</v>
       </c>
       <c r="H21" s="25"/>
       <c r="I21" s="25"/>
-      <c r="J21" s="95"/>
-      <c r="K21" s="51" t="s">
+      <c r="J21" s="94"/>
+      <c r="K21" s="50" t="s">
         <v>18</v>
       </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
-      <c r="N21" s="95"/>
-      <c r="O21" s="51" t="s">
+      <c r="N21" s="94"/>
+      <c r="O21" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="P21" s="52"/>
-      <c r="Q21" s="52"/>
-      <c r="R21" s="106"/>
+      <c r="P21" s="51"/>
+      <c r="Q21" s="51"/>
+      <c r="R21" s="104"/>
       <c r="S21" s="20"/>
     </row>
     <row r="22" spans="2:19" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="190" t="s">
+      <c r="B22" s="199" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="56" t="s">
+      <c r="C22" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="55"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="57"/>
-      <c r="O22" s="57"/>
-      <c r="P22" s="57"/>
-      <c r="Q22" s="57"/>
-      <c r="R22" s="107"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="56"/>
+      <c r="Q22" s="56"/>
+      <c r="R22" s="105"/>
     </row>
     <row r="23" spans="2:19" s="23" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="191"/>
-      <c r="C23" s="58" t="s">
+      <c r="B23" s="200"/>
+      <c r="C23" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="176" t="s">
+      <c r="D23" s="185" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="177"/>
-      <c r="F23" s="177"/>
-      <c r="G23" s="177"/>
-      <c r="H23" s="177"/>
-      <c r="I23" s="177"/>
-      <c r="J23" s="177"/>
-      <c r="K23" s="177"/>
-      <c r="L23" s="177"/>
-      <c r="M23" s="177"/>
-      <c r="N23" s="177"/>
-      <c r="O23" s="177"/>
-      <c r="P23" s="178"/>
-      <c r="Q23" s="167" t="s">
+      <c r="E23" s="186"/>
+      <c r="F23" s="186"/>
+      <c r="G23" s="186"/>
+      <c r="H23" s="186"/>
+      <c r="I23" s="186"/>
+      <c r="J23" s="186"/>
+      <c r="K23" s="186"/>
+      <c r="L23" s="186"/>
+      <c r="M23" s="186"/>
+      <c r="N23" s="186"/>
+      <c r="O23" s="186"/>
+      <c r="P23" s="187"/>
+      <c r="Q23" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="R23" s="168"/>
+      <c r="R23" s="177"/>
     </row>
     <row r="24" spans="2:19" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="191"/>
-      <c r="C24" s="113"/>
-      <c r="D24" s="223"/>
-      <c r="E24" s="118"/>
-      <c r="F24" s="118"/>
-      <c r="G24" s="118"/>
-      <c r="H24" s="118"/>
-      <c r="I24" s="118"/>
-      <c r="J24" s="118"/>
-      <c r="K24" s="118"/>
-      <c r="L24" s="118"/>
-      <c r="M24" s="118"/>
-      <c r="N24" s="118"/>
-      <c r="O24" s="118"/>
-      <c r="P24" s="59"/>
-      <c r="Q24" s="224"/>
-      <c r="R24" s="225"/>
+      <c r="B24" s="200"/>
+      <c r="C24" s="110"/>
+      <c r="D24" s="121"/>
+      <c r="E24" s="122"/>
+      <c r="F24" s="122"/>
+      <c r="G24" s="122"/>
+      <c r="H24" s="122"/>
+      <c r="I24" s="122"/>
+      <c r="J24" s="122"/>
+      <c r="K24" s="122"/>
+      <c r="L24" s="122"/>
+      <c r="M24" s="122"/>
+      <c r="N24" s="122"/>
+      <c r="O24" s="122"/>
+      <c r="P24" s="58"/>
+      <c r="Q24" s="119"/>
+      <c r="R24" s="120"/>
     </row>
     <row r="25" spans="2:19" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="191"/>
-      <c r="C25" s="113"/>
-      <c r="D25" s="223"/>
-      <c r="E25" s="118"/>
-      <c r="F25" s="118"/>
-      <c r="G25" s="118"/>
-      <c r="H25" s="118"/>
-      <c r="I25" s="118"/>
-      <c r="J25" s="118"/>
-      <c r="K25" s="118"/>
-      <c r="L25" s="118"/>
-      <c r="M25" s="118"/>
-      <c r="N25" s="118"/>
-      <c r="O25" s="118"/>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="224"/>
-      <c r="R25" s="225"/>
+      <c r="B25" s="200"/>
+      <c r="C25" s="110"/>
+      <c r="D25" s="121"/>
+      <c r="E25" s="122"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="122"/>
+      <c r="H25" s="122"/>
+      <c r="I25" s="122"/>
+      <c r="J25" s="122"/>
+      <c r="K25" s="122"/>
+      <c r="L25" s="122"/>
+      <c r="M25" s="122"/>
+      <c r="N25" s="122"/>
+      <c r="O25" s="122"/>
+      <c r="P25" s="58"/>
+      <c r="Q25" s="119"/>
+      <c r="R25" s="120"/>
     </row>
     <row r="26" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="191"/>
-      <c r="C26" s="114"/>
-      <c r="D26" s="223"/>
-      <c r="E26" s="118"/>
-      <c r="F26" s="118"/>
-      <c r="G26" s="118"/>
-      <c r="H26" s="118"/>
-      <c r="I26" s="118"/>
-      <c r="J26" s="118"/>
-      <c r="K26" s="118"/>
-      <c r="L26" s="118"/>
-      <c r="M26" s="118"/>
-      <c r="N26" s="118"/>
-      <c r="O26" s="118"/>
-      <c r="P26" s="60"/>
-      <c r="Q26" s="224"/>
-      <c r="R26" s="225"/>
+      <c r="B26" s="200"/>
+      <c r="C26" s="111"/>
+      <c r="D26" s="121"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="122"/>
+      <c r="I26" s="122"/>
+      <c r="J26" s="122"/>
+      <c r="K26" s="122"/>
+      <c r="L26" s="122"/>
+      <c r="M26" s="122"/>
+      <c r="N26" s="122"/>
+      <c r="O26" s="122"/>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="119"/>
+      <c r="R26" s="120"/>
     </row>
     <row r="27" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="191"/>
-      <c r="C27" s="114"/>
-      <c r="D27" s="223"/>
-      <c r="E27" s="118"/>
-      <c r="F27" s="118"/>
-      <c r="G27" s="118"/>
-      <c r="H27" s="118"/>
-      <c r="I27" s="118"/>
-      <c r="J27" s="118"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="118"/>
-      <c r="M27" s="118"/>
-      <c r="N27" s="118"/>
-      <c r="O27" s="118"/>
-      <c r="P27" s="60"/>
-      <c r="Q27" s="224"/>
-      <c r="R27" s="225"/>
+      <c r="B27" s="200"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="121"/>
+      <c r="E27" s="122"/>
+      <c r="F27" s="122"/>
+      <c r="G27" s="122"/>
+      <c r="H27" s="122"/>
+      <c r="I27" s="122"/>
+      <c r="J27" s="122"/>
+      <c r="K27" s="122"/>
+      <c r="L27" s="122"/>
+      <c r="M27" s="122"/>
+      <c r="N27" s="122"/>
+      <c r="O27" s="122"/>
+      <c r="P27" s="59"/>
+      <c r="Q27" s="119"/>
+      <c r="R27" s="120"/>
     </row>
     <row r="28" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="191"/>
-      <c r="C28" s="114"/>
-      <c r="D28" s="223"/>
-      <c r="E28" s="118"/>
-      <c r="F28" s="118"/>
-      <c r="G28" s="118"/>
-      <c r="H28" s="118"/>
-      <c r="I28" s="118"/>
-      <c r="J28" s="118"/>
-      <c r="K28" s="118"/>
-      <c r="L28" s="118"/>
-      <c r="M28" s="118"/>
-      <c r="N28" s="118"/>
-      <c r="O28" s="118"/>
-      <c r="P28" s="60"/>
-      <c r="Q28" s="224"/>
-      <c r="R28" s="225"/>
+      <c r="B28" s="200"/>
+      <c r="C28" s="111"/>
+      <c r="D28" s="121"/>
+      <c r="E28" s="122"/>
+      <c r="F28" s="122"/>
+      <c r="G28" s="122"/>
+      <c r="H28" s="122"/>
+      <c r="I28" s="122"/>
+      <c r="J28" s="122"/>
+      <c r="K28" s="122"/>
+      <c r="L28" s="122"/>
+      <c r="M28" s="122"/>
+      <c r="N28" s="122"/>
+      <c r="O28" s="122"/>
+      <c r="P28" s="59"/>
+      <c r="Q28" s="119"/>
+      <c r="R28" s="120"/>
     </row>
     <row r="29" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="191"/>
-      <c r="C29" s="114"/>
-      <c r="D29" s="223"/>
-      <c r="E29" s="118"/>
-      <c r="F29" s="118"/>
-      <c r="G29" s="118"/>
-      <c r="H29" s="118"/>
-      <c r="I29" s="118"/>
-      <c r="J29" s="118"/>
-      <c r="K29" s="118"/>
-      <c r="L29" s="118"/>
-      <c r="M29" s="118"/>
-      <c r="N29" s="118"/>
-      <c r="O29" s="118"/>
-      <c r="P29" s="60"/>
-      <c r="Q29" s="224"/>
-      <c r="R29" s="225"/>
+      <c r="B29" s="200"/>
+      <c r="C29" s="111"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="122"/>
+      <c r="F29" s="122"/>
+      <c r="G29" s="122"/>
+      <c r="H29" s="122"/>
+      <c r="I29" s="122"/>
+      <c r="J29" s="122"/>
+      <c r="K29" s="122"/>
+      <c r="L29" s="122"/>
+      <c r="M29" s="122"/>
+      <c r="N29" s="122"/>
+      <c r="O29" s="122"/>
+      <c r="P29" s="59"/>
+      <c r="Q29" s="119"/>
+      <c r="R29" s="120"/>
     </row>
     <row r="30" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="191"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="223"/>
-      <c r="E30" s="118"/>
-      <c r="F30" s="118"/>
-      <c r="G30" s="118"/>
-      <c r="H30" s="118"/>
-      <c r="I30" s="118"/>
-      <c r="J30" s="118"/>
-      <c r="K30" s="118"/>
-      <c r="L30" s="118"/>
-      <c r="M30" s="118"/>
-      <c r="N30" s="118"/>
-      <c r="O30" s="118"/>
-      <c r="P30" s="60"/>
-      <c r="Q30" s="224"/>
-      <c r="R30" s="225"/>
+      <c r="B30" s="200"/>
+      <c r="C30" s="111"/>
+      <c r="D30" s="121"/>
+      <c r="E30" s="122"/>
+      <c r="F30" s="122"/>
+      <c r="G30" s="122"/>
+      <c r="H30" s="122"/>
+      <c r="I30" s="122"/>
+      <c r="J30" s="122"/>
+      <c r="K30" s="122"/>
+      <c r="L30" s="122"/>
+      <c r="M30" s="122"/>
+      <c r="N30" s="122"/>
+      <c r="O30" s="122"/>
+      <c r="P30" s="59"/>
+      <c r="Q30" s="119"/>
+      <c r="R30" s="120"/>
     </row>
     <row r="31" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="191"/>
-      <c r="C31" s="114"/>
-      <c r="D31" s="223"/>
-      <c r="E31" s="118"/>
-      <c r="F31" s="118"/>
-      <c r="G31" s="118"/>
-      <c r="H31" s="118"/>
-      <c r="I31" s="118"/>
-      <c r="J31" s="118"/>
-      <c r="K31" s="118"/>
-      <c r="L31" s="118"/>
-      <c r="M31" s="118"/>
-      <c r="N31" s="118"/>
-      <c r="O31" s="118"/>
-      <c r="P31" s="60"/>
-      <c r="Q31" s="224"/>
-      <c r="R31" s="225"/>
+      <c r="B31" s="200"/>
+      <c r="C31" s="111"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="122"/>
+      <c r="F31" s="122"/>
+      <c r="G31" s="122"/>
+      <c r="H31" s="122"/>
+      <c r="I31" s="122"/>
+      <c r="J31" s="122"/>
+      <c r="K31" s="122"/>
+      <c r="L31" s="122"/>
+      <c r="M31" s="122"/>
+      <c r="N31" s="122"/>
+      <c r="O31" s="122"/>
+      <c r="P31" s="59"/>
+      <c r="Q31" s="119"/>
+      <c r="R31" s="120"/>
     </row>
     <row r="32" spans="2:19" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="191"/>
-      <c r="C32" s="206" t="s">
+      <c r="B32" s="200"/>
+      <c r="C32" s="215" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="207"/>
-      <c r="E32" s="207"/>
-      <c r="F32" s="207"/>
-      <c r="G32" s="207"/>
-      <c r="H32" s="207"/>
-      <c r="I32" s="207"/>
-      <c r="J32" s="207"/>
-      <c r="K32" s="207"/>
-      <c r="L32" s="207"/>
-      <c r="M32" s="207"/>
-      <c r="N32" s="207"/>
-      <c r="O32" s="208"/>
-      <c r="P32" s="126" t="s">
+      <c r="D32" s="216"/>
+      <c r="E32" s="216"/>
+      <c r="F32" s="216"/>
+      <c r="G32" s="216"/>
+      <c r="H32" s="216"/>
+      <c r="I32" s="216"/>
+      <c r="J32" s="216"/>
+      <c r="K32" s="216"/>
+      <c r="L32" s="216"/>
+      <c r="M32" s="216"/>
+      <c r="N32" s="216"/>
+      <c r="O32" s="217"/>
+      <c r="P32" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="Q32" s="128"/>
-      <c r="R32" s="129"/>
+      <c r="Q32" s="133"/>
+      <c r="R32" s="134"/>
     </row>
     <row r="33" spans="2:20" s="19" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="191"/>
-      <c r="C33" s="209" t="s">
+      <c r="B33" s="200"/>
+      <c r="C33" s="218" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="210"/>
-      <c r="E33" s="210"/>
-      <c r="F33" s="210"/>
-      <c r="G33" s="210"/>
-      <c r="H33" s="210"/>
-      <c r="I33" s="210"/>
-      <c r="J33" s="210"/>
-      <c r="K33" s="210"/>
-      <c r="L33" s="210"/>
-      <c r="M33" s="210"/>
-      <c r="N33" s="210"/>
-      <c r="O33" s="211"/>
-      <c r="P33" s="127"/>
-      <c r="Q33" s="130"/>
-      <c r="R33" s="131"/>
+      <c r="D33" s="219"/>
+      <c r="E33" s="219"/>
+      <c r="F33" s="219"/>
+      <c r="G33" s="219"/>
+      <c r="H33" s="219"/>
+      <c r="I33" s="219"/>
+      <c r="J33" s="219"/>
+      <c r="K33" s="219"/>
+      <c r="L33" s="219"/>
+      <c r="M33" s="219"/>
+      <c r="N33" s="219"/>
+      <c r="O33" s="220"/>
+      <c r="P33" s="132"/>
+      <c r="Q33" s="135"/>
+      <c r="R33" s="136"/>
     </row>
     <row r="34" spans="2:20" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="191"/>
-      <c r="C34" s="61" t="s">
+      <c r="B34" s="200"/>
+      <c r="C34" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="94"/>
-      <c r="H34" s="94"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="62"/>
-      <c r="K34" s="62"/>
-      <c r="L34" s="108"/>
-      <c r="M34" s="62"/>
-      <c r="N34" s="62"/>
-      <c r="O34" s="62"/>
-      <c r="P34" s="62"/>
-      <c r="Q34" s="62"/>
-      <c r="R34" s="63"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="93"/>
+      <c r="H34" s="93"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
+      <c r="L34" s="106"/>
+      <c r="M34" s="61"/>
+      <c r="N34" s="61"/>
+      <c r="O34" s="61"/>
+      <c r="P34" s="61"/>
+      <c r="Q34" s="61"/>
+      <c r="R34" s="62"/>
     </row>
     <row r="35" spans="2:20" s="20" customFormat="1" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="191"/>
-      <c r="C35" s="100" t="s">
+      <c r="B35" s="200"/>
+      <c r="C35" s="98" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="67"/>
-      <c r="L35" s="67"/>
-      <c r="M35" s="67"/>
-      <c r="N35" s="67"/>
-      <c r="O35" s="67"/>
-      <c r="P35" s="67"/>
-      <c r="Q35" s="67"/>
-      <c r="R35" s="66"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="66"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="66"/>
+      <c r="J35" s="66"/>
+      <c r="K35" s="66"/>
+      <c r="L35" s="66"/>
+      <c r="M35" s="66"/>
+      <c r="N35" s="66"/>
+      <c r="O35" s="66"/>
+      <c r="P35" s="66"/>
+      <c r="Q35" s="66"/>
+      <c r="R35" s="65"/>
     </row>
     <row r="36" spans="2:20" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="203" t="s">
+      <c r="B36" s="212" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="198" t="s">
+      <c r="C36" s="207" t="s">
         <v>41</v>
       </c>
-      <c r="D36" s="199"/>
-      <c r="E36" s="199"/>
-      <c r="F36" s="200"/>
-      <c r="G36" s="122"/>
-      <c r="H36" s="123"/>
-      <c r="I36" s="68"/>
-      <c r="J36" s="68"/>
-      <c r="K36" s="68"/>
-      <c r="L36" s="68"/>
-      <c r="M36" s="68"/>
-      <c r="N36" s="68"/>
-      <c r="O36" s="68"/>
-      <c r="P36" s="68"/>
-      <c r="Q36" s="68"/>
-      <c r="R36" s="69"/>
+      <c r="D36" s="208"/>
+      <c r="E36" s="208"/>
+      <c r="F36" s="209"/>
+      <c r="G36" s="127"/>
+      <c r="H36" s="128"/>
+      <c r="I36" s="67"/>
+      <c r="J36" s="67"/>
+      <c r="K36" s="67"/>
+      <c r="L36" s="67"/>
+      <c r="M36" s="67"/>
+      <c r="N36" s="67"/>
+      <c r="O36" s="67"/>
+      <c r="P36" s="67"/>
+      <c r="Q36" s="67"/>
+      <c r="R36" s="68"/>
     </row>
     <row r="37" spans="2:20" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="204"/>
-      <c r="C37" s="201"/>
-      <c r="D37" s="202"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="71"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="70"/>
-      <c r="K37" s="70"/>
-      <c r="L37" s="70"/>
-      <c r="M37" s="70"/>
-      <c r="N37" s="70"/>
-      <c r="O37" s="72"/>
-      <c r="P37" s="72"/>
-      <c r="Q37" s="72"/>
-      <c r="R37" s="73"/>
+      <c r="B37" s="213"/>
+      <c r="C37" s="210"/>
+      <c r="D37" s="211"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="69"/>
+      <c r="K37" s="69"/>
+      <c r="L37" s="69"/>
+      <c r="M37" s="69"/>
+      <c r="N37" s="69"/>
+      <c r="O37" s="71"/>
+      <c r="P37" s="71"/>
+      <c r="Q37" s="71"/>
+      <c r="R37" s="72"/>
     </row>
     <row r="38" spans="2:20" s="20" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="204"/>
-      <c r="C38" s="201"/>
-      <c r="D38" s="202"/>
-      <c r="E38" s="192" t="s">
+      <c r="B38" s="213"/>
+      <c r="C38" s="210"/>
+      <c r="D38" s="211"/>
+      <c r="E38" s="201" t="s">
         <v>64</v>
       </c>
-      <c r="F38" s="193"/>
-      <c r="G38" s="198" t="s">
+      <c r="F38" s="202"/>
+      <c r="G38" s="207" t="s">
         <v>55</v>
       </c>
-      <c r="H38" s="199"/>
-      <c r="I38" s="199"/>
-      <c r="J38" s="199"/>
-      <c r="K38" s="199"/>
-      <c r="L38" s="199"/>
-      <c r="M38" s="199"/>
-      <c r="N38" s="199"/>
-      <c r="O38" s="200"/>
-      <c r="P38" s="219"/>
-      <c r="Q38" s="219"/>
-      <c r="R38" s="220"/>
+      <c r="H38" s="208"/>
+      <c r="I38" s="208"/>
+      <c r="J38" s="208"/>
+      <c r="K38" s="208"/>
+      <c r="L38" s="208"/>
+      <c r="M38" s="208"/>
+      <c r="N38" s="208"/>
+      <c r="O38" s="209"/>
+      <c r="P38" s="160"/>
+      <c r="Q38" s="160"/>
+      <c r="R38" s="161"/>
     </row>
     <row r="39" spans="2:20" s="20" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="204"/>
-      <c r="C39" s="201"/>
-      <c r="D39" s="202"/>
-      <c r="E39" s="194"/>
-      <c r="F39" s="195"/>
-      <c r="G39" s="90" t="s">
+      <c r="B39" s="213"/>
+      <c r="C39" s="210"/>
+      <c r="D39" s="211"/>
+      <c r="E39" s="203"/>
+      <c r="F39" s="204"/>
+      <c r="G39" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="H39" s="91" t="s">
+      <c r="H39" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="I39" s="91" t="s">
+      <c r="I39" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="J39" s="91" t="s">
+      <c r="J39" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="K39" s="91" t="s">
+      <c r="K39" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="L39" s="91" t="s">
+      <c r="L39" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="M39" s="91" t="s">
+      <c r="M39" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="N39" s="91" t="s">
+      <c r="N39" s="90" t="s">
         <v>49</v>
       </c>
-      <c r="O39" s="92" t="s">
+      <c r="O39" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="P39" s="219"/>
-      <c r="Q39" s="219"/>
-      <c r="R39" s="220"/>
+      <c r="P39" s="160"/>
+      <c r="Q39" s="160"/>
+      <c r="R39" s="161"/>
     </row>
     <row r="40" spans="2:20" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="204"/>
-      <c r="C40" s="201"/>
-      <c r="D40" s="202"/>
-      <c r="E40" s="196"/>
-      <c r="F40" s="197"/>
-      <c r="G40" s="109"/>
-      <c r="H40" s="110"/>
-      <c r="I40" s="110"/>
-      <c r="J40" s="110"/>
-      <c r="K40" s="110"/>
-      <c r="L40" s="110"/>
-      <c r="M40" s="110"/>
-      <c r="N40" s="110"/>
-      <c r="O40" s="111"/>
-      <c r="P40" s="219"/>
-      <c r="Q40" s="219"/>
-      <c r="R40" s="220"/>
+      <c r="B40" s="213"/>
+      <c r="C40" s="210"/>
+      <c r="D40" s="211"/>
+      <c r="E40" s="205"/>
+      <c r="F40" s="206"/>
+      <c r="G40" s="107"/>
+      <c r="H40" s="108"/>
+      <c r="I40" s="108"/>
+      <c r="J40" s="108"/>
+      <c r="K40" s="108"/>
+      <c r="L40" s="108"/>
+      <c r="M40" s="108"/>
+      <c r="N40" s="108"/>
+      <c r="O40" s="109"/>
+      <c r="P40" s="160"/>
+      <c r="Q40" s="160"/>
+      <c r="R40" s="161"/>
     </row>
     <row r="41" spans="2:20" s="20" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="204"/>
-      <c r="C41" s="74"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
-      <c r="G41" s="77"/>
-      <c r="H41" s="77"/>
-      <c r="I41" s="77"/>
-      <c r="J41" s="77"/>
-      <c r="K41" s="77"/>
-      <c r="L41" s="77"/>
-      <c r="M41" s="77"/>
-      <c r="N41" s="77"/>
-      <c r="O41" s="77"/>
-      <c r="P41" s="78"/>
-      <c r="Q41" s="78"/>
-      <c r="R41" s="79"/>
+      <c r="B41" s="213"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="75"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+      <c r="J41" s="76"/>
+      <c r="K41" s="76"/>
+      <c r="L41" s="76"/>
+      <c r="M41" s="76"/>
+      <c r="N41" s="76"/>
+      <c r="O41" s="76"/>
+      <c r="P41" s="77"/>
+      <c r="Q41" s="77"/>
+      <c r="R41" s="78"/>
     </row>
     <row r="42" spans="2:20" s="20" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="204"/>
-      <c r="C42" s="221" t="s">
+      <c r="B42" s="213"/>
+      <c r="C42" s="162" t="s">
         <v>56</v>
       </c>
-      <c r="D42" s="222"/>
-      <c r="E42" s="222"/>
-      <c r="F42" s="80" t="s">
+      <c r="D42" s="163"/>
+      <c r="E42" s="163"/>
+      <c r="F42" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="G42" s="80"/>
-      <c r="H42" s="80"/>
-      <c r="I42" s="80"/>
-      <c r="J42" s="80"/>
-      <c r="K42" s="124" t="s">
+      <c r="G42" s="79"/>
+      <c r="H42" s="79"/>
+      <c r="I42" s="79"/>
+      <c r="J42" s="79"/>
+      <c r="K42" s="129" t="s">
         <v>63</v>
       </c>
-      <c r="L42" s="124"/>
-      <c r="M42" s="124"/>
-      <c r="N42" s="124"/>
-      <c r="O42" s="124"/>
-      <c r="P42" s="124"/>
-      <c r="Q42" s="124"/>
-      <c r="R42" s="125"/>
+      <c r="L42" s="129"/>
+      <c r="M42" s="129"/>
+      <c r="N42" s="129"/>
+      <c r="O42" s="129"/>
+      <c r="P42" s="129"/>
+      <c r="Q42" s="129"/>
+      <c r="R42" s="130"/>
     </row>
     <row r="43" spans="2:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="204"/>
-      <c r="C43" s="212" t="s">
+      <c r="B43" s="213"/>
+      <c r="C43" s="221" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="213"/>
-      <c r="E43" s="213"/>
-      <c r="F43" s="213" t="s">
+      <c r="D43" s="222"/>
+      <c r="E43" s="222"/>
+      <c r="F43" s="222" t="s">
         <v>62</v>
       </c>
-      <c r="G43" s="213"/>
-      <c r="H43" s="213"/>
-      <c r="I43" s="213"/>
-      <c r="J43" s="213"/>
-      <c r="K43" s="215" t="s">
+      <c r="G43" s="222"/>
+      <c r="H43" s="222"/>
+      <c r="I43" s="222"/>
+      <c r="J43" s="222"/>
+      <c r="K43" s="224" t="s">
         <v>59</v>
       </c>
-      <c r="L43" s="215"/>
-      <c r="M43" s="215"/>
-      <c r="N43" s="215"/>
-      <c r="O43" s="215"/>
-      <c r="P43" s="215"/>
-      <c r="Q43" s="215"/>
-      <c r="R43" s="217"/>
+      <c r="L43" s="224"/>
+      <c r="M43" s="224"/>
+      <c r="N43" s="224"/>
+      <c r="O43" s="224"/>
+      <c r="P43" s="224"/>
+      <c r="Q43" s="224"/>
+      <c r="R43" s="226"/>
     </row>
     <row r="44" spans="2:20" s="20" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="204"/>
-      <c r="C44" s="214" t="s">
+      <c r="B44" s="213"/>
+      <c r="C44" s="223" t="s">
         <v>83</v>
       </c>
-      <c r="D44" s="215"/>
-      <c r="E44" s="215"/>
-      <c r="F44" s="216" t="s">
+      <c r="D44" s="224"/>
+      <c r="E44" s="224"/>
+      <c r="F44" s="225" t="s">
         <v>58</v>
       </c>
-      <c r="G44" s="216"/>
-      <c r="H44" s="216"/>
-      <c r="I44" s="216"/>
-      <c r="J44" s="216"/>
-      <c r="K44" s="213" t="s">
+      <c r="G44" s="225"/>
+      <c r="H44" s="225"/>
+      <c r="I44" s="225"/>
+      <c r="J44" s="225"/>
+      <c r="K44" s="222" t="s">
         <v>60</v>
       </c>
-      <c r="L44" s="213"/>
-      <c r="M44" s="213"/>
-      <c r="N44" s="213"/>
-      <c r="O44" s="213"/>
-      <c r="P44" s="213"/>
-      <c r="Q44" s="213"/>
-      <c r="R44" s="218"/>
+      <c r="L44" s="222"/>
+      <c r="M44" s="222"/>
+      <c r="N44" s="222"/>
+      <c r="O44" s="222"/>
+      <c r="P44" s="222"/>
+      <c r="Q44" s="222"/>
+      <c r="R44" s="227"/>
     </row>
     <row r="45" spans="2:20" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="204"/>
-      <c r="C45" s="101"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="81"/>
-      <c r="G45" s="81"/>
-      <c r="H45" s="81"/>
-      <c r="I45" s="81"/>
-      <c r="J45" s="81"/>
-      <c r="K45" s="81"/>
-      <c r="L45" s="81"/>
-      <c r="M45" s="81"/>
-      <c r="N45" s="81"/>
-      <c r="O45" s="99"/>
-      <c r="P45" s="82"/>
-      <c r="Q45" s="82"/>
-      <c r="R45" s="83"/>
+      <c r="B45" s="213"/>
+      <c r="C45" s="99"/>
+      <c r="D45" s="80"/>
+      <c r="E45" s="80"/>
+      <c r="F45" s="80"/>
+      <c r="G45" s="80"/>
+      <c r="H45" s="80"/>
+      <c r="I45" s="80"/>
+      <c r="J45" s="80"/>
+      <c r="K45" s="80"/>
+      <c r="L45" s="80"/>
+      <c r="M45" s="80"/>
+      <c r="N45" s="80"/>
+      <c r="O45" s="97"/>
+      <c r="P45" s="81"/>
+      <c r="Q45" s="81"/>
+      <c r="R45" s="82"/>
       <c r="S45" s="20"/>
       <c r="T45" s="20"/>
     </row>
     <row r="46" spans="2:20" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="204"/>
-      <c r="C46" s="103"/>
-      <c r="D46" s="104" t="s">
+      <c r="B46" s="213"/>
+      <c r="C46" s="101"/>
+      <c r="D46" s="102" t="s">
         <v>81</v>
       </c>
-      <c r="E46" s="84"/>
-      <c r="F46" s="84"/>
-      <c r="G46" s="84"/>
-      <c r="H46" s="84"/>
-      <c r="I46" s="84"/>
-      <c r="J46" s="84"/>
-      <c r="K46" s="84"/>
-      <c r="L46" s="104" t="s">
+      <c r="E46" s="83"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="83"/>
+      <c r="H46" s="83"/>
+      <c r="I46" s="83"/>
+      <c r="J46" s="83"/>
+      <c r="K46" s="83"/>
+      <c r="L46" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="M46" s="77"/>
-      <c r="N46" s="84"/>
-      <c r="O46" s="98"/>
-      <c r="P46" s="85"/>
-      <c r="Q46" s="85"/>
-      <c r="R46" s="86"/>
+      <c r="M46" s="76"/>
+      <c r="N46" s="83"/>
+      <c r="O46" s="96"/>
+      <c r="P46" s="84"/>
+      <c r="Q46" s="84"/>
+      <c r="R46" s="85"/>
       <c r="S46" s="20"/>
     </row>
     <row r="47" spans="2:20" s="4" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="205"/>
-      <c r="C47" s="102"/>
-      <c r="D47" s="87"/>
-      <c r="E47" s="87"/>
-      <c r="F47" s="87"/>
-      <c r="G47" s="87"/>
-      <c r="H47" s="87"/>
-      <c r="I47" s="87"/>
-      <c r="J47" s="87"/>
-      <c r="K47" s="87"/>
-      <c r="L47" s="87"/>
-      <c r="M47" s="87"/>
-      <c r="N47" s="87"/>
-      <c r="O47" s="97"/>
-      <c r="P47" s="88"/>
-      <c r="Q47" s="88"/>
-      <c r="R47" s="89"/>
+      <c r="B47" s="214"/>
+      <c r="C47" s="100"/>
+      <c r="D47" s="86"/>
+      <c r="E47" s="86"/>
+      <c r="F47" s="86"/>
+      <c r="G47" s="86"/>
+      <c r="H47" s="86"/>
+      <c r="I47" s="86"/>
+      <c r="J47" s="86"/>
+      <c r="K47" s="86"/>
+      <c r="L47" s="86"/>
+      <c r="M47" s="86"/>
+      <c r="N47" s="86"/>
+      <c r="O47" s="95"/>
+      <c r="P47" s="87"/>
+      <c r="Q47" s="87"/>
+      <c r="R47" s="88"/>
       <c r="S47" s="20"/>
     </row>
     <row r="48" spans="2:20" s="4" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="152"/>
-      <c r="D48" s="153"/>
-      <c r="E48" s="153"/>
-      <c r="F48" s="153"/>
-      <c r="G48" s="153"/>
-      <c r="H48" s="153"/>
-      <c r="I48" s="153"/>
-      <c r="J48" s="153"/>
-      <c r="K48" s="153"/>
-      <c r="L48" s="153"/>
-      <c r="M48" s="153"/>
-      <c r="N48" s="153"/>
-      <c r="O48" s="153"/>
-      <c r="P48" s="153"/>
-      <c r="Q48" s="153"/>
-      <c r="R48" s="154"/>
+      <c r="C48" s="157"/>
+      <c r="D48" s="158"/>
+      <c r="E48" s="158"/>
+      <c r="F48" s="158"/>
+      <c r="G48" s="158"/>
+      <c r="H48" s="158"/>
+      <c r="I48" s="158"/>
+      <c r="J48" s="158"/>
+      <c r="K48" s="158"/>
+      <c r="L48" s="158"/>
+      <c r="M48" s="158"/>
+      <c r="N48" s="158"/>
+      <c r="O48" s="158"/>
+      <c r="P48" s="158"/>
+      <c r="Q48" s="158"/>
+      <c r="R48" s="159"/>
       <c r="S48" s="20"/>
     </row>
     <row r="49" spans="2:19" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="26"/>
-      <c r="C49" s="132" t="s">
+      <c r="C49" s="137" t="s">
         <v>70</v>
       </c>
-      <c r="D49" s="133"/>
-      <c r="E49" s="133"/>
-      <c r="F49" s="133"/>
-      <c r="G49" s="134"/>
-      <c r="H49" s="138" t="s">
+      <c r="D49" s="138"/>
+      <c r="E49" s="138"/>
+      <c r="F49" s="138"/>
+      <c r="G49" s="139"/>
+      <c r="H49" s="143" t="s">
         <v>78</v>
       </c>
-      <c r="I49" s="133"/>
-      <c r="J49" s="133"/>
-      <c r="K49" s="133"/>
-      <c r="L49" s="134"/>
-      <c r="M49" s="140" t="s">
+      <c r="I49" s="138"/>
+      <c r="J49" s="138"/>
+      <c r="K49" s="138"/>
+      <c r="L49" s="139"/>
+      <c r="M49" s="145" t="s">
         <v>68</v>
       </c>
-      <c r="N49" s="141"/>
-      <c r="O49" s="142"/>
-      <c r="P49" s="140" t="s">
+      <c r="N49" s="146"/>
+      <c r="O49" s="147"/>
+      <c r="P49" s="145" t="s">
         <v>69</v>
       </c>
-      <c r="Q49" s="141"/>
-      <c r="R49" s="149"/>
+      <c r="Q49" s="146"/>
+      <c r="R49" s="154"/>
       <c r="S49" s="20"/>
     </row>
     <row r="50" spans="2:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C50" s="135"/>
-      <c r="D50" s="136"/>
-      <c r="E50" s="136"/>
-      <c r="F50" s="136"/>
-      <c r="G50" s="137"/>
-      <c r="H50" s="139"/>
-      <c r="I50" s="136"/>
-      <c r="J50" s="136"/>
-      <c r="K50" s="136"/>
-      <c r="L50" s="137"/>
-      <c r="M50" s="143"/>
-      <c r="N50" s="144"/>
-      <c r="O50" s="145"/>
-      <c r="P50" s="143"/>
-      <c r="Q50" s="144"/>
-      <c r="R50" s="150"/>
+      <c r="C50" s="140"/>
+      <c r="D50" s="141"/>
+      <c r="E50" s="141"/>
+      <c r="F50" s="141"/>
+      <c r="G50" s="142"/>
+      <c r="H50" s="144"/>
+      <c r="I50" s="141"/>
+      <c r="J50" s="141"/>
+      <c r="K50" s="141"/>
+      <c r="L50" s="142"/>
+      <c r="M50" s="148"/>
+      <c r="N50" s="149"/>
+      <c r="O50" s="150"/>
+      <c r="P50" s="148"/>
+      <c r="Q50" s="149"/>
+      <c r="R50" s="155"/>
       <c r="S50" s="20"/>
     </row>
     <row r="51" spans="2:19" s="5" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="53" t="s">
+      <c r="C51" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D51" s="46"/>
-      <c r="E51" s="46"/>
-      <c r="F51" s="46"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="54" t="s">
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="I51" s="46"/>
-      <c r="J51" s="46"/>
-      <c r="K51" s="46"/>
-      <c r="L51" s="46"/>
-      <c r="M51" s="146"/>
-      <c r="N51" s="147"/>
-      <c r="O51" s="148"/>
-      <c r="P51" s="146"/>
-      <c r="Q51" s="147"/>
-      <c r="R51" s="151"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="228"/>
+      <c r="K51" s="229"/>
+      <c r="L51" s="45"/>
+      <c r="M51" s="151"/>
+      <c r="N51" s="152"/>
+      <c r="O51" s="153"/>
+      <c r="P51" s="151"/>
+      <c r="Q51" s="152"/>
+      <c r="R51" s="156"/>
       <c r="S51" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="N11:R11"/>
-    <mergeCell ref="D25:O25"/>
-    <mergeCell ref="D26:O26"/>
-    <mergeCell ref="D27:O27"/>
-    <mergeCell ref="D29:O29"/>
-    <mergeCell ref="D28:O28"/>
     <mergeCell ref="B22:B35"/>
     <mergeCell ref="E38:F40"/>
     <mergeCell ref="G38:O38"/>
@@ -3923,8 +3909,8 @@
     <mergeCell ref="F44:J44"/>
     <mergeCell ref="K43:R43"/>
     <mergeCell ref="K44:R44"/>
-    <mergeCell ref="P38:R40"/>
-    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="D25:O25"/>
+    <mergeCell ref="D26:O26"/>
     <mergeCell ref="C4:H5"/>
     <mergeCell ref="I4:R5"/>
     <mergeCell ref="Q23:R23"/>
@@ -3932,15 +3918,15 @@
     <mergeCell ref="G17:N17"/>
     <mergeCell ref="O17:R17"/>
     <mergeCell ref="D23:P23"/>
-    <mergeCell ref="N6:R6"/>
     <mergeCell ref="O19:Q19"/>
     <mergeCell ref="O20:Q20"/>
     <mergeCell ref="F8:R8"/>
     <mergeCell ref="F9:L9"/>
     <mergeCell ref="F10:L10"/>
     <mergeCell ref="F11:L11"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="N11:R11"/>
     <mergeCell ref="F12:L12"/>
-    <mergeCell ref="F13:L13"/>
     <mergeCell ref="K42:R42"/>
     <mergeCell ref="P32:P33"/>
     <mergeCell ref="Q32:R33"/>
@@ -3949,20 +3935,27 @@
     <mergeCell ref="M49:O51"/>
     <mergeCell ref="P49:R51"/>
     <mergeCell ref="C48:R48"/>
+    <mergeCell ref="P38:R40"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="J51:K51"/>
     <mergeCell ref="F7:L7"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="G36:H36"/>
     <mergeCell ref="D30:O30"/>
     <mergeCell ref="D31:O31"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="D29:O29"/>
+    <mergeCell ref="D28:O28"/>
+    <mergeCell ref="D27:O27"/>
+    <mergeCell ref="F13:L13"/>
     <mergeCell ref="Q28:R28"/>
     <mergeCell ref="Q29:R29"/>
     <mergeCell ref="Q30:R30"/>
     <mergeCell ref="Q31:R31"/>
     <mergeCell ref="D24:O24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
ISP20220996  - Check List 新增CheckEMB選項
</commit_message>
<xml_diff>
--- a/Quality/Quality/XLT/InspBySPQuery_Detail.xlsx
+++ b/Quality/Quality/XLT/InspBySPQuery_Detail.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Inspection Report '!$B$1:$R$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Inspection Report '!$B$1:$R$54</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="89">
   <si>
     <t>TOTAL</t>
   </si>
@@ -713,6 +713,14 @@
   </si>
   <si>
     <t>Sample Type</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">EMB </t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Printing/AOP</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
 </sst>
@@ -1872,6 +1880,252 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1954,252 +2208,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="9"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="9"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2224,13 +2232,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2238,7 +2246,7 @@
         <xdr:cNvPr id="4108" name="AutoShape 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C100000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C100000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2297,7 +2305,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2333,13 +2341,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>428609</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>11902</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>352409</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>142871</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2347,7 +2355,7 @@
         <xdr:cNvPr id="5" name="AutoShape 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2766,10 +2774,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T52"/>
+  <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2793,42 +2801,42 @@
     <row r="1" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:20" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="150"/>
-      <c r="D4" s="151"/>
-      <c r="E4" s="151"/>
-      <c r="F4" s="151"/>
-      <c r="G4" s="151"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="156" t="s">
+      <c r="C4" s="169"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
+      <c r="F4" s="170"/>
+      <c r="G4" s="170"/>
+      <c r="H4" s="171"/>
+      <c r="I4" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="157"/>
-      <c r="K4" s="157"/>
-      <c r="L4" s="157"/>
-      <c r="M4" s="157"/>
-      <c r="N4" s="157"/>
-      <c r="O4" s="157"/>
-      <c r="P4" s="157"/>
-      <c r="Q4" s="157"/>
-      <c r="R4" s="158"/>
+      <c r="J4" s="176"/>
+      <c r="K4" s="176"/>
+      <c r="L4" s="176"/>
+      <c r="M4" s="176"/>
+      <c r="N4" s="176"/>
+      <c r="O4" s="176"/>
+      <c r="P4" s="176"/>
+      <c r="Q4" s="176"/>
+      <c r="R4" s="177"/>
     </row>
     <row r="5" spans="1:20" ht="10.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="153"/>
-      <c r="D5" s="154"/>
-      <c r="E5" s="154"/>
-      <c r="F5" s="154"/>
-      <c r="G5" s="154"/>
-      <c r="H5" s="155"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="160"/>
-      <c r="K5" s="160"/>
-      <c r="L5" s="160"/>
-      <c r="M5" s="160"/>
-      <c r="N5" s="160"/>
-      <c r="O5" s="160"/>
-      <c r="P5" s="160"/>
-      <c r="Q5" s="160"/>
-      <c r="R5" s="161"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="173"/>
+      <c r="E5" s="173"/>
+      <c r="F5" s="173"/>
+      <c r="G5" s="173"/>
+      <c r="H5" s="174"/>
+      <c r="I5" s="178"/>
+      <c r="J5" s="179"/>
+      <c r="K5" s="179"/>
+      <c r="L5" s="179"/>
+      <c r="M5" s="179"/>
+      <c r="N5" s="179"/>
+      <c r="O5" s="179"/>
+      <c r="P5" s="179"/>
+      <c r="Q5" s="179"/>
+      <c r="R5" s="180"/>
     </row>
     <row r="6" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="7" t="s">
@@ -2844,11 +2852,11 @@
         <v>65</v>
       </c>
       <c r="I6" s="92"/>
-      <c r="J6" s="165" t="s">
+      <c r="J6" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="224"/>
-      <c r="L6" s="225"/>
+      <c r="K6" s="125"/>
+      <c r="L6" s="126"/>
       <c r="M6" s="29" t="s">
         <v>80</v>
       </c>
@@ -2867,13 +2875,13 @@
       <c r="E7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="184"/>
-      <c r="G7" s="149"/>
-      <c r="H7" s="149"/>
-      <c r="I7" s="149"/>
-      <c r="J7" s="149"/>
-      <c r="K7" s="149"/>
-      <c r="L7" s="149"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="122"/>
+      <c r="I7" s="122"/>
+      <c r="J7" s="122"/>
+      <c r="K7" s="122"/>
+      <c r="L7" s="122"/>
       <c r="M7" s="11"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -2892,19 +2900,19 @@
       <c r="E8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="181"/>
-      <c r="G8" s="182"/>
-      <c r="H8" s="182"/>
-      <c r="I8" s="182"/>
-      <c r="J8" s="182"/>
-      <c r="K8" s="182"/>
-      <c r="L8" s="182"/>
-      <c r="M8" s="182"/>
-      <c r="N8" s="182"/>
-      <c r="O8" s="182"/>
-      <c r="P8" s="182"/>
-      <c r="Q8" s="182"/>
-      <c r="R8" s="183"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="130"/>
+      <c r="H8" s="130"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="130"/>
+      <c r="K8" s="130"/>
+      <c r="L8" s="130"/>
+      <c r="M8" s="130"/>
+      <c r="N8" s="130"/>
+      <c r="O8" s="130"/>
+      <c r="P8" s="130"/>
+      <c r="Q8" s="130"/>
+      <c r="R8" s="131"/>
       <c r="S8" s="20"/>
     </row>
     <row r="9" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2917,19 +2925,19 @@
       <c r="E9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="181"/>
-      <c r="G9" s="182"/>
-      <c r="H9" s="182"/>
-      <c r="I9" s="182"/>
-      <c r="J9" s="182"/>
-      <c r="K9" s="182"/>
-      <c r="L9" s="182"/>
-      <c r="M9" s="182"/>
-      <c r="N9" s="182"/>
-      <c r="O9" s="182"/>
-      <c r="P9" s="182"/>
-      <c r="Q9" s="182"/>
-      <c r="R9" s="183"/>
+      <c r="F9" s="129"/>
+      <c r="G9" s="130"/>
+      <c r="H9" s="130"/>
+      <c r="I9" s="130"/>
+      <c r="J9" s="130"/>
+      <c r="K9" s="130"/>
+      <c r="L9" s="130"/>
+      <c r="M9" s="130"/>
+      <c r="N9" s="130"/>
+      <c r="O9" s="130"/>
+      <c r="P9" s="130"/>
+      <c r="Q9" s="130"/>
+      <c r="R9" s="131"/>
       <c r="S9" s="20"/>
     </row>
     <row r="10" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2940,21 +2948,21 @@
       <c r="E10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="184"/>
-      <c r="G10" s="149"/>
-      <c r="H10" s="149"/>
-      <c r="I10" s="149"/>
-      <c r="J10" s="149"/>
-      <c r="K10" s="149"/>
-      <c r="L10" s="149"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="122"/>
+      <c r="I10" s="122"/>
+      <c r="J10" s="122"/>
+      <c r="K10" s="122"/>
+      <c r="L10" s="122"/>
       <c r="M10" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="N10" s="184"/>
-      <c r="O10" s="185"/>
-      <c r="P10" s="185"/>
-      <c r="Q10" s="185"/>
-      <c r="R10" s="186"/>
+      <c r="N10" s="123"/>
+      <c r="O10" s="199"/>
+      <c r="P10" s="199"/>
+      <c r="Q10" s="199"/>
+      <c r="R10" s="200"/>
       <c r="S10" s="112"/>
       <c r="T10" s="116"/>
     </row>
@@ -2966,13 +2974,13 @@
       <c r="E11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="184"/>
-      <c r="G11" s="149"/>
-      <c r="H11" s="149"/>
-      <c r="I11" s="149"/>
-      <c r="J11" s="149"/>
-      <c r="K11" s="149"/>
-      <c r="L11" s="149"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="122"/>
+      <c r="H11" s="122"/>
+      <c r="I11" s="122"/>
+      <c r="J11" s="122"/>
+      <c r="K11" s="122"/>
+      <c r="L11" s="122"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -2989,21 +2997,21 @@
       <c r="E12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="184"/>
-      <c r="G12" s="149"/>
-      <c r="H12" s="149"/>
-      <c r="I12" s="149"/>
-      <c r="J12" s="149"/>
-      <c r="K12" s="149"/>
-      <c r="L12" s="149"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="122"/>
+      <c r="H12" s="122"/>
+      <c r="I12" s="122"/>
+      <c r="J12" s="122"/>
+      <c r="K12" s="122"/>
+      <c r="L12" s="122"/>
       <c r="M12" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="N12" s="184"/>
-      <c r="O12" s="185"/>
-      <c r="P12" s="185"/>
-      <c r="Q12" s="185"/>
-      <c r="R12" s="186"/>
+      <c r="N12" s="123"/>
+      <c r="O12" s="199"/>
+      <c r="P12" s="199"/>
+      <c r="Q12" s="199"/>
+      <c r="R12" s="200"/>
       <c r="S12" s="112"/>
       <c r="T12" s="112"/>
     </row>
@@ -3015,13 +3023,13 @@
       <c r="E13" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="184"/>
-      <c r="G13" s="149"/>
-      <c r="H13" s="149"/>
-      <c r="I13" s="149"/>
-      <c r="J13" s="149"/>
-      <c r="K13" s="149"/>
-      <c r="L13" s="149"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="122"/>
+      <c r="I13" s="122"/>
+      <c r="J13" s="122"/>
+      <c r="K13" s="122"/>
+      <c r="L13" s="122"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -3038,13 +3046,13 @@
       <c r="E14" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="F14" s="184"/>
-      <c r="G14" s="149"/>
-      <c r="H14" s="149"/>
-      <c r="I14" s="149"/>
-      <c r="J14" s="149"/>
-      <c r="K14" s="149"/>
-      <c r="L14" s="149"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="122"/>
+      <c r="H14" s="122"/>
+      <c r="I14" s="122"/>
+      <c r="J14" s="122"/>
+      <c r="K14" s="122"/>
+      <c r="L14" s="122"/>
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
       <c r="O14" s="25"/>
@@ -3131,28 +3139,28 @@
       <c r="S17" s="20"/>
     </row>
     <row r="18" spans="2:19" s="16" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="164" t="s">
+      <c r="C18" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="165"/>
-      <c r="E18" s="165"/>
-      <c r="F18" s="166"/>
-      <c r="G18" s="167" t="s">
+      <c r="D18" s="124"/>
+      <c r="E18" s="124"/>
+      <c r="F18" s="184"/>
+      <c r="G18" s="185" t="s">
         <v>77</v>
       </c>
-      <c r="H18" s="168"/>
-      <c r="I18" s="168"/>
-      <c r="J18" s="168"/>
-      <c r="K18" s="168"/>
-      <c r="L18" s="168"/>
-      <c r="M18" s="168"/>
-      <c r="N18" s="168"/>
-      <c r="O18" s="169" t="s">
+      <c r="H18" s="186"/>
+      <c r="I18" s="186"/>
+      <c r="J18" s="186"/>
+      <c r="K18" s="186"/>
+      <c r="L18" s="186"/>
+      <c r="M18" s="186"/>
+      <c r="N18" s="186"/>
+      <c r="O18" s="187" t="s">
         <v>13</v>
       </c>
-      <c r="P18" s="170"/>
-      <c r="Q18" s="170"/>
-      <c r="R18" s="171"/>
+      <c r="P18" s="188"/>
+      <c r="Q18" s="188"/>
+      <c r="R18" s="189"/>
       <c r="S18" s="22"/>
     </row>
     <row r="19" spans="2:19" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3203,11 +3211,11 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="94"/>
-      <c r="O20" s="175" t="s">
+      <c r="O20" s="193" t="s">
         <v>74</v>
       </c>
-      <c r="P20" s="176"/>
-      <c r="Q20" s="177"/>
+      <c r="P20" s="194"/>
+      <c r="Q20" s="195"/>
       <c r="R20" s="104"/>
       <c r="S20" s="20"/>
     </row>
@@ -3232,17 +3240,17 @@
         <v>73</v>
       </c>
       <c r="N21" s="94"/>
-      <c r="O21" s="178" t="s">
+      <c r="O21" s="196" t="s">
         <v>36</v>
       </c>
-      <c r="P21" s="179"/>
-      <c r="Q21" s="180"/>
+      <c r="P21" s="197"/>
+      <c r="Q21" s="198"/>
       <c r="R21" s="104"/>
       <c r="S21" s="103"/>
     </row>
-    <row r="22" spans="2:19" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="48" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D22" s="49"/>
       <c r="E22" s="25"/>
@@ -3267,700 +3275,728 @@
       <c r="R22" s="104"/>
       <c r="S22" s="20"/>
     </row>
-    <row r="23" spans="2:19" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="119" t="s">
+    <row r="23" spans="2:19" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="49"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="94"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="94"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="104"/>
+      <c r="S23" s="20"/>
+    </row>
+    <row r="24" spans="2:19" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="49"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="94"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="94"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="51"/>
+      <c r="R24" s="104"/>
+      <c r="S24" s="20"/>
+    </row>
+    <row r="25" spans="2:19" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="55" t="s">
+      <c r="C25" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="54"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="56"/>
-      <c r="P23" s="56"/>
-      <c r="Q23" s="56"/>
-      <c r="R23" s="105"/>
-    </row>
-    <row r="24" spans="2:19" s="23" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="120"/>
-      <c r="C24" s="57" t="s">
+      <c r="D25" s="54"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="56"/>
+      <c r="P25" s="56"/>
+      <c r="Q25" s="56"/>
+      <c r="R25" s="105"/>
+    </row>
+    <row r="26" spans="2:19" s="23" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="202"/>
+      <c r="C26" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="172" t="s">
+      <c r="D26" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="173"/>
-      <c r="F24" s="173"/>
-      <c r="G24" s="173"/>
-      <c r="H24" s="173"/>
-      <c r="I24" s="173"/>
-      <c r="J24" s="173"/>
-      <c r="K24" s="173"/>
-      <c r="L24" s="173"/>
-      <c r="M24" s="173"/>
-      <c r="N24" s="173"/>
-      <c r="O24" s="173"/>
-      <c r="P24" s="174"/>
-      <c r="Q24" s="162" t="s">
+      <c r="E26" s="191"/>
+      <c r="F26" s="191"/>
+      <c r="G26" s="191"/>
+      <c r="H26" s="191"/>
+      <c r="I26" s="191"/>
+      <c r="J26" s="191"/>
+      <c r="K26" s="191"/>
+      <c r="L26" s="191"/>
+      <c r="M26" s="191"/>
+      <c r="N26" s="191"/>
+      <c r="O26" s="191"/>
+      <c r="P26" s="192"/>
+      <c r="Q26" s="181" t="s">
         <v>14</v>
       </c>
-      <c r="R24" s="163"/>
-    </row>
-    <row r="25" spans="2:19" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="120"/>
-      <c r="C25" s="110"/>
-      <c r="D25" s="148"/>
-      <c r="E25" s="149"/>
-      <c r="F25" s="149"/>
-      <c r="G25" s="149"/>
-      <c r="H25" s="149"/>
-      <c r="I25" s="149"/>
-      <c r="J25" s="149"/>
-      <c r="K25" s="149"/>
-      <c r="L25" s="149"/>
-      <c r="M25" s="149"/>
-      <c r="N25" s="149"/>
-      <c r="O25" s="149"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="228"/>
-      <c r="R25" s="229"/>
-    </row>
-    <row r="26" spans="2:19" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="120"/>
-      <c r="C26" s="110"/>
-      <c r="D26" s="148"/>
-      <c r="E26" s="149"/>
-      <c r="F26" s="149"/>
-      <c r="G26" s="149"/>
-      <c r="H26" s="149"/>
-      <c r="I26" s="149"/>
-      <c r="J26" s="149"/>
-      <c r="K26" s="149"/>
-      <c r="L26" s="149"/>
-      <c r="M26" s="149"/>
-      <c r="N26" s="149"/>
-      <c r="O26" s="149"/>
-      <c r="P26" s="58"/>
-      <c r="Q26" s="228"/>
-      <c r="R26" s="229"/>
-    </row>
-    <row r="27" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="120"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="148"/>
-      <c r="E27" s="149"/>
-      <c r="F27" s="149"/>
-      <c r="G27" s="149"/>
-      <c r="H27" s="149"/>
-      <c r="I27" s="149"/>
-      <c r="J27" s="149"/>
-      <c r="K27" s="149"/>
-      <c r="L27" s="149"/>
-      <c r="M27" s="149"/>
-      <c r="N27" s="149"/>
-      <c r="O27" s="149"/>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="228"/>
-      <c r="R27" s="229"/>
-    </row>
-    <row r="28" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="120"/>
-      <c r="C28" s="111"/>
-      <c r="D28" s="148"/>
-      <c r="E28" s="149"/>
-      <c r="F28" s="149"/>
-      <c r="G28" s="149"/>
-      <c r="H28" s="149"/>
-      <c r="I28" s="149"/>
-      <c r="J28" s="149"/>
-      <c r="K28" s="149"/>
-      <c r="L28" s="149"/>
-      <c r="M28" s="149"/>
-      <c r="N28" s="149"/>
-      <c r="O28" s="149"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="228"/>
-      <c r="R28" s="229"/>
+      <c r="R26" s="182"/>
+    </row>
+    <row r="27" spans="2:19" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="202"/>
+      <c r="C27" s="110"/>
+      <c r="D27" s="121"/>
+      <c r="E27" s="122"/>
+      <c r="F27" s="122"/>
+      <c r="G27" s="122"/>
+      <c r="H27" s="122"/>
+      <c r="I27" s="122"/>
+      <c r="J27" s="122"/>
+      <c r="K27" s="122"/>
+      <c r="L27" s="122"/>
+      <c r="M27" s="122"/>
+      <c r="N27" s="122"/>
+      <c r="O27" s="122"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="119"/>
+      <c r="R27" s="120"/>
+    </row>
+    <row r="28" spans="2:19" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="202"/>
+      <c r="C28" s="110"/>
+      <c r="D28" s="121"/>
+      <c r="E28" s="122"/>
+      <c r="F28" s="122"/>
+      <c r="G28" s="122"/>
+      <c r="H28" s="122"/>
+      <c r="I28" s="122"/>
+      <c r="J28" s="122"/>
+      <c r="K28" s="122"/>
+      <c r="L28" s="122"/>
+      <c r="M28" s="122"/>
+      <c r="N28" s="122"/>
+      <c r="O28" s="122"/>
+      <c r="P28" s="58"/>
+      <c r="Q28" s="119"/>
+      <c r="R28" s="120"/>
     </row>
     <row r="29" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="120"/>
+      <c r="B29" s="202"/>
       <c r="C29" s="111"/>
-      <c r="D29" s="148"/>
-      <c r="E29" s="149"/>
-      <c r="F29" s="149"/>
-      <c r="G29" s="149"/>
-      <c r="H29" s="149"/>
-      <c r="I29" s="149"/>
-      <c r="J29" s="149"/>
-      <c r="K29" s="149"/>
-      <c r="L29" s="149"/>
-      <c r="M29" s="149"/>
-      <c r="N29" s="149"/>
-      <c r="O29" s="149"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="122"/>
+      <c r="F29" s="122"/>
+      <c r="G29" s="122"/>
+      <c r="H29" s="122"/>
+      <c r="I29" s="122"/>
+      <c r="J29" s="122"/>
+      <c r="K29" s="122"/>
+      <c r="L29" s="122"/>
+      <c r="M29" s="122"/>
+      <c r="N29" s="122"/>
+      <c r="O29" s="122"/>
       <c r="P29" s="59"/>
-      <c r="Q29" s="228"/>
-      <c r="R29" s="229"/>
+      <c r="Q29" s="119"/>
+      <c r="R29" s="120"/>
     </row>
     <row r="30" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="120"/>
+      <c r="B30" s="202"/>
       <c r="C30" s="111"/>
-      <c r="D30" s="148"/>
-      <c r="E30" s="149"/>
-      <c r="F30" s="149"/>
-      <c r="G30" s="149"/>
-      <c r="H30" s="149"/>
-      <c r="I30" s="149"/>
-      <c r="J30" s="149"/>
-      <c r="K30" s="149"/>
-      <c r="L30" s="149"/>
-      <c r="M30" s="149"/>
-      <c r="N30" s="149"/>
-      <c r="O30" s="149"/>
+      <c r="D30" s="121"/>
+      <c r="E30" s="122"/>
+      <c r="F30" s="122"/>
+      <c r="G30" s="122"/>
+      <c r="H30" s="122"/>
+      <c r="I30" s="122"/>
+      <c r="J30" s="122"/>
+      <c r="K30" s="122"/>
+      <c r="L30" s="122"/>
+      <c r="M30" s="122"/>
+      <c r="N30" s="122"/>
+      <c r="O30" s="122"/>
       <c r="P30" s="59"/>
-      <c r="Q30" s="228"/>
-      <c r="R30" s="229"/>
+      <c r="Q30" s="119"/>
+      <c r="R30" s="120"/>
     </row>
     <row r="31" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="120"/>
+      <c r="B31" s="202"/>
       <c r="C31" s="111"/>
-      <c r="D31" s="148"/>
-      <c r="E31" s="149"/>
-      <c r="F31" s="149"/>
-      <c r="G31" s="149"/>
-      <c r="H31" s="149"/>
-      <c r="I31" s="149"/>
-      <c r="J31" s="149"/>
-      <c r="K31" s="149"/>
-      <c r="L31" s="149"/>
-      <c r="M31" s="149"/>
-      <c r="N31" s="149"/>
-      <c r="O31" s="149"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="122"/>
+      <c r="F31" s="122"/>
+      <c r="G31" s="122"/>
+      <c r="H31" s="122"/>
+      <c r="I31" s="122"/>
+      <c r="J31" s="122"/>
+      <c r="K31" s="122"/>
+      <c r="L31" s="122"/>
+      <c r="M31" s="122"/>
+      <c r="N31" s="122"/>
+      <c r="O31" s="122"/>
       <c r="P31" s="59"/>
-      <c r="Q31" s="228"/>
-      <c r="R31" s="229"/>
+      <c r="Q31" s="119"/>
+      <c r="R31" s="120"/>
     </row>
     <row r="32" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="120"/>
+      <c r="B32" s="202"/>
       <c r="C32" s="111"/>
-      <c r="D32" s="148"/>
-      <c r="E32" s="149"/>
-      <c r="F32" s="149"/>
-      <c r="G32" s="149"/>
-      <c r="H32" s="149"/>
-      <c r="I32" s="149"/>
-      <c r="J32" s="149"/>
-      <c r="K32" s="149"/>
-      <c r="L32" s="149"/>
-      <c r="M32" s="149"/>
-      <c r="N32" s="149"/>
-      <c r="O32" s="149"/>
+      <c r="D32" s="121"/>
+      <c r="E32" s="122"/>
+      <c r="F32" s="122"/>
+      <c r="G32" s="122"/>
+      <c r="H32" s="122"/>
+      <c r="I32" s="122"/>
+      <c r="J32" s="122"/>
+      <c r="K32" s="122"/>
+      <c r="L32" s="122"/>
+      <c r="M32" s="122"/>
+      <c r="N32" s="122"/>
+      <c r="O32" s="122"/>
       <c r="P32" s="59"/>
-      <c r="Q32" s="228"/>
-      <c r="R32" s="229"/>
-    </row>
-    <row r="33" spans="2:20" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="120"/>
-      <c r="C33" s="135" t="s">
+      <c r="Q32" s="119"/>
+      <c r="R32" s="120"/>
+    </row>
+    <row r="33" spans="2:20" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="202"/>
+      <c r="C33" s="111"/>
+      <c r="D33" s="121"/>
+      <c r="E33" s="122"/>
+      <c r="F33" s="122"/>
+      <c r="G33" s="122"/>
+      <c r="H33" s="122"/>
+      <c r="I33" s="122"/>
+      <c r="J33" s="122"/>
+      <c r="K33" s="122"/>
+      <c r="L33" s="122"/>
+      <c r="M33" s="122"/>
+      <c r="N33" s="122"/>
+      <c r="O33" s="122"/>
+      <c r="P33" s="59"/>
+      <c r="Q33" s="119"/>
+      <c r="R33" s="120"/>
+    </row>
+    <row r="34" spans="2:20" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="202"/>
+      <c r="C34" s="111"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="122"/>
+      <c r="F34" s="122"/>
+      <c r="G34" s="122"/>
+      <c r="H34" s="122"/>
+      <c r="I34" s="122"/>
+      <c r="J34" s="122"/>
+      <c r="K34" s="122"/>
+      <c r="L34" s="122"/>
+      <c r="M34" s="122"/>
+      <c r="N34" s="122"/>
+      <c r="O34" s="122"/>
+      <c r="P34" s="59"/>
+      <c r="Q34" s="119"/>
+      <c r="R34" s="120"/>
+    </row>
+    <row r="35" spans="2:20" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="202"/>
+      <c r="C35" s="217" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="136"/>
-      <c r="E33" s="136"/>
-      <c r="F33" s="136"/>
-      <c r="G33" s="136"/>
-      <c r="H33" s="136"/>
-      <c r="I33" s="136"/>
-      <c r="J33" s="136"/>
-      <c r="K33" s="136"/>
-      <c r="L33" s="136"/>
-      <c r="M33" s="136"/>
-      <c r="N33" s="136"/>
-      <c r="O33" s="137"/>
-      <c r="P33" s="189" t="s">
+      <c r="D35" s="218"/>
+      <c r="E35" s="218"/>
+      <c r="F35" s="218"/>
+      <c r="G35" s="218"/>
+      <c r="H35" s="218"/>
+      <c r="I35" s="218"/>
+      <c r="J35" s="218"/>
+      <c r="K35" s="218"/>
+      <c r="L35" s="218"/>
+      <c r="M35" s="218"/>
+      <c r="N35" s="218"/>
+      <c r="O35" s="219"/>
+      <c r="P35" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="Q33" s="191"/>
-      <c r="R33" s="192"/>
-    </row>
-    <row r="34" spans="2:20" s="19" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="120"/>
-      <c r="C34" s="138" t="s">
+      <c r="Q35" s="136"/>
+      <c r="R35" s="137"/>
+    </row>
+    <row r="36" spans="2:20" s="19" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="202"/>
+      <c r="C36" s="220" t="s">
         <v>54</v>
       </c>
-      <c r="D34" s="139"/>
-      <c r="E34" s="139"/>
-      <c r="F34" s="139"/>
-      <c r="G34" s="139"/>
-      <c r="H34" s="139"/>
-      <c r="I34" s="139"/>
-      <c r="J34" s="139"/>
-      <c r="K34" s="139"/>
-      <c r="L34" s="139"/>
-      <c r="M34" s="139"/>
-      <c r="N34" s="139"/>
-      <c r="O34" s="140"/>
-      <c r="P34" s="190"/>
-      <c r="Q34" s="193"/>
-      <c r="R34" s="194"/>
-    </row>
-    <row r="35" spans="2:20" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="120"/>
-      <c r="C35" s="60" t="s">
+      <c r="D36" s="221"/>
+      <c r="E36" s="221"/>
+      <c r="F36" s="221"/>
+      <c r="G36" s="221"/>
+      <c r="H36" s="221"/>
+      <c r="I36" s="221"/>
+      <c r="J36" s="221"/>
+      <c r="K36" s="221"/>
+      <c r="L36" s="221"/>
+      <c r="M36" s="221"/>
+      <c r="N36" s="221"/>
+      <c r="O36" s="222"/>
+      <c r="P36" s="135"/>
+      <c r="Q36" s="138"/>
+      <c r="R36" s="139"/>
+    </row>
+    <row r="37" spans="2:20" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="202"/>
+      <c r="C37" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="93"/>
-      <c r="H35" s="93"/>
-      <c r="I35" s="61"/>
-      <c r="J35" s="61"/>
-      <c r="K35" s="61"/>
-      <c r="L35" s="106"/>
-      <c r="M35" s="61"/>
-      <c r="N35" s="61"/>
-      <c r="O35" s="61"/>
-      <c r="P35" s="61"/>
-      <c r="Q35" s="61"/>
-      <c r="R35" s="62"/>
-    </row>
-    <row r="36" spans="2:20" s="20" customFormat="1" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="120"/>
-      <c r="C36" s="98" t="s">
+      <c r="D37" s="61"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="93"/>
+      <c r="H37" s="93"/>
+      <c r="I37" s="61"/>
+      <c r="J37" s="61"/>
+      <c r="K37" s="61"/>
+      <c r="L37" s="106"/>
+      <c r="M37" s="61"/>
+      <c r="N37" s="61"/>
+      <c r="O37" s="61"/>
+      <c r="P37" s="61"/>
+      <c r="Q37" s="61"/>
+      <c r="R37" s="62"/>
+    </row>
+    <row r="38" spans="2:20" s="20" customFormat="1" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="202"/>
+      <c r="C38" s="98" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="66"/>
-      <c r="H36" s="66"/>
-      <c r="I36" s="66"/>
-      <c r="J36" s="66"/>
-      <c r="K36" s="66"/>
-      <c r="L36" s="66"/>
-      <c r="M36" s="66"/>
-      <c r="N36" s="66"/>
-      <c r="O36" s="66"/>
-      <c r="P36" s="66"/>
-      <c r="Q36" s="66"/>
-      <c r="R36" s="65"/>
-    </row>
-    <row r="37" spans="2:20" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="132" t="s">
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="66"/>
+      <c r="H38" s="66"/>
+      <c r="I38" s="66"/>
+      <c r="J38" s="66"/>
+      <c r="K38" s="66"/>
+      <c r="L38" s="66"/>
+      <c r="M38" s="66"/>
+      <c r="N38" s="66"/>
+      <c r="O38" s="66"/>
+      <c r="P38" s="66"/>
+      <c r="Q38" s="66"/>
+      <c r="R38" s="65"/>
+    </row>
+    <row r="39" spans="2:20" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="127" t="s">
+      <c r="C39" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="D37" s="128"/>
-      <c r="E37" s="128"/>
-      <c r="F37" s="129"/>
-      <c r="G37" s="226"/>
-      <c r="H37" s="227"/>
-      <c r="I37" s="67"/>
-      <c r="J37" s="67"/>
-      <c r="K37" s="67"/>
-      <c r="L37" s="67"/>
-      <c r="M37" s="67"/>
-      <c r="N37" s="67"/>
-      <c r="O37" s="67"/>
-      <c r="P37" s="67"/>
-      <c r="Q37" s="67"/>
-      <c r="R37" s="68"/>
-    </row>
-    <row r="38" spans="2:20" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="133"/>
-      <c r="C38" s="130"/>
-      <c r="D38" s="131"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="69"/>
-      <c r="G38" s="70"/>
-      <c r="H38" s="70"/>
-      <c r="I38" s="69"/>
-      <c r="J38" s="69"/>
-      <c r="K38" s="69"/>
-      <c r="L38" s="69"/>
-      <c r="M38" s="69"/>
-      <c r="N38" s="69"/>
-      <c r="O38" s="71"/>
-      <c r="P38" s="71"/>
-      <c r="Q38" s="71"/>
-      <c r="R38" s="72"/>
-    </row>
-    <row r="39" spans="2:20" s="20" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="133"/>
-      <c r="C39" s="130"/>
-      <c r="D39" s="131"/>
-      <c r="E39" s="121" t="s">
+      <c r="D39" s="210"/>
+      <c r="E39" s="210"/>
+      <c r="F39" s="211"/>
+      <c r="G39" s="127"/>
+      <c r="H39" s="128"/>
+      <c r="I39" s="67"/>
+      <c r="J39" s="67"/>
+      <c r="K39" s="67"/>
+      <c r="L39" s="67"/>
+      <c r="M39" s="67"/>
+      <c r="N39" s="67"/>
+      <c r="O39" s="67"/>
+      <c r="P39" s="67"/>
+      <c r="Q39" s="67"/>
+      <c r="R39" s="68"/>
+    </row>
+    <row r="40" spans="2:20" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="215"/>
+      <c r="C40" s="212"/>
+      <c r="D40" s="213"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="70"/>
+      <c r="I40" s="69"/>
+      <c r="J40" s="69"/>
+      <c r="K40" s="69"/>
+      <c r="L40" s="69"/>
+      <c r="M40" s="69"/>
+      <c r="N40" s="69"/>
+      <c r="O40" s="71"/>
+      <c r="P40" s="71"/>
+      <c r="Q40" s="71"/>
+      <c r="R40" s="72"/>
+    </row>
+    <row r="41" spans="2:20" s="20" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="215"/>
+      <c r="C41" s="212"/>
+      <c r="D41" s="213"/>
+      <c r="E41" s="203" t="s">
         <v>64</v>
       </c>
-      <c r="F39" s="122"/>
-      <c r="G39" s="127" t="s">
+      <c r="F41" s="204"/>
+      <c r="G41" s="209" t="s">
         <v>55</v>
       </c>
-      <c r="H39" s="128"/>
-      <c r="I39" s="128"/>
-      <c r="J39" s="128"/>
-      <c r="K39" s="128"/>
-      <c r="L39" s="128"/>
-      <c r="M39" s="128"/>
-      <c r="N39" s="128"/>
-      <c r="O39" s="129"/>
-      <c r="P39" s="218"/>
-      <c r="Q39" s="218"/>
-      <c r="R39" s="219"/>
-    </row>
-    <row r="40" spans="2:20" s="20" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="133"/>
-      <c r="C40" s="130"/>
-      <c r="D40" s="131"/>
-      <c r="E40" s="123"/>
-      <c r="F40" s="124"/>
-      <c r="G40" s="89" t="s">
+      <c r="H41" s="210"/>
+      <c r="I41" s="210"/>
+      <c r="J41" s="210"/>
+      <c r="K41" s="210"/>
+      <c r="L41" s="210"/>
+      <c r="M41" s="210"/>
+      <c r="N41" s="210"/>
+      <c r="O41" s="211"/>
+      <c r="P41" s="163"/>
+      <c r="Q41" s="163"/>
+      <c r="R41" s="164"/>
+    </row>
+    <row r="42" spans="2:20" s="20" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="215"/>
+      <c r="C42" s="212"/>
+      <c r="D42" s="213"/>
+      <c r="E42" s="205"/>
+      <c r="F42" s="206"/>
+      <c r="G42" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="H40" s="90" t="s">
+      <c r="H42" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="I40" s="90" t="s">
+      <c r="I42" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="J40" s="90" t="s">
+      <c r="J42" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="K40" s="90" t="s">
+      <c r="K42" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="L40" s="90" t="s">
+      <c r="L42" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="M40" s="90" t="s">
+      <c r="M42" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="N40" s="90" t="s">
+      <c r="N42" s="90" t="s">
         <v>49</v>
       </c>
-      <c r="O40" s="91" t="s">
+      <c r="O42" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="P40" s="218"/>
-      <c r="Q40" s="218"/>
-      <c r="R40" s="219"/>
-    </row>
-    <row r="41" spans="2:20" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="133"/>
-      <c r="C41" s="130"/>
-      <c r="D41" s="131"/>
-      <c r="E41" s="125"/>
-      <c r="F41" s="126"/>
-      <c r="G41" s="107"/>
-      <c r="H41" s="108"/>
-      <c r="I41" s="108"/>
-      <c r="J41" s="108"/>
-      <c r="K41" s="108"/>
-      <c r="L41" s="108"/>
-      <c r="M41" s="108"/>
-      <c r="N41" s="108"/>
-      <c r="O41" s="109"/>
-      <c r="P41" s="218"/>
-      <c r="Q41" s="218"/>
-      <c r="R41" s="219"/>
-    </row>
-    <row r="42" spans="2:20" s="20" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="133"/>
-      <c r="C42" s="73"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="75"/>
-      <c r="F42" s="75"/>
-      <c r="G42" s="76"/>
-      <c r="H42" s="76"/>
-      <c r="I42" s="76"/>
-      <c r="J42" s="76"/>
-      <c r="K42" s="76"/>
-      <c r="L42" s="76"/>
-      <c r="M42" s="76"/>
-      <c r="N42" s="76"/>
-      <c r="O42" s="76"/>
-      <c r="P42" s="77"/>
-      <c r="Q42" s="77"/>
-      <c r="R42" s="78"/>
-    </row>
-    <row r="43" spans="2:20" s="20" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="133"/>
-      <c r="C43" s="220" t="s">
+      <c r="P42" s="163"/>
+      <c r="Q42" s="163"/>
+      <c r="R42" s="164"/>
+    </row>
+    <row r="43" spans="2:20" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="215"/>
+      <c r="C43" s="212"/>
+      <c r="D43" s="213"/>
+      <c r="E43" s="207"/>
+      <c r="F43" s="208"/>
+      <c r="G43" s="107"/>
+      <c r="H43" s="108"/>
+      <c r="I43" s="108"/>
+      <c r="J43" s="108"/>
+      <c r="K43" s="108"/>
+      <c r="L43" s="108"/>
+      <c r="M43" s="108"/>
+      <c r="N43" s="108"/>
+      <c r="O43" s="109"/>
+      <c r="P43" s="163"/>
+      <c r="Q43" s="163"/>
+      <c r="R43" s="164"/>
+    </row>
+    <row r="44" spans="2:20" s="20" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="215"/>
+      <c r="C44" s="73"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="75"/>
+      <c r="F44" s="75"/>
+      <c r="G44" s="76"/>
+      <c r="H44" s="76"/>
+      <c r="I44" s="76"/>
+      <c r="J44" s="76"/>
+      <c r="K44" s="76"/>
+      <c r="L44" s="76"/>
+      <c r="M44" s="76"/>
+      <c r="N44" s="76"/>
+      <c r="O44" s="76"/>
+      <c r="P44" s="77"/>
+      <c r="Q44" s="77"/>
+      <c r="R44" s="78"/>
+    </row>
+    <row r="45" spans="2:20" s="20" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="215"/>
+      <c r="C45" s="165" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="221"/>
-      <c r="E43" s="221"/>
-      <c r="F43" s="79" t="s">
+      <c r="D45" s="166"/>
+      <c r="E45" s="166"/>
+      <c r="F45" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="G43" s="79"/>
-      <c r="H43" s="79"/>
-      <c r="I43" s="79"/>
-      <c r="J43" s="79"/>
-      <c r="K43" s="187" t="s">
+      <c r="G45" s="79"/>
+      <c r="H45" s="79"/>
+      <c r="I45" s="79"/>
+      <c r="J45" s="79"/>
+      <c r="K45" s="132" t="s">
         <v>63</v>
       </c>
-      <c r="L43" s="187"/>
-      <c r="M43" s="187"/>
-      <c r="N43" s="187"/>
-      <c r="O43" s="187"/>
-      <c r="P43" s="187"/>
-      <c r="Q43" s="187"/>
-      <c r="R43" s="188"/>
-    </row>
-    <row r="44" spans="2:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="133"/>
-      <c r="C44" s="141" t="s">
+      <c r="L45" s="132"/>
+      <c r="M45" s="132"/>
+      <c r="N45" s="132"/>
+      <c r="O45" s="132"/>
+      <c r="P45" s="132"/>
+      <c r="Q45" s="132"/>
+      <c r="R45" s="133"/>
+    </row>
+    <row r="46" spans="2:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="215"/>
+      <c r="C46" s="223" t="s">
         <v>61</v>
       </c>
-      <c r="D44" s="142"/>
-      <c r="E44" s="142"/>
-      <c r="F44" s="142" t="s">
+      <c r="D46" s="224"/>
+      <c r="E46" s="224"/>
+      <c r="F46" s="224" t="s">
         <v>62</v>
       </c>
-      <c r="G44" s="142"/>
-      <c r="H44" s="142"/>
-      <c r="I44" s="142"/>
-      <c r="J44" s="142"/>
-      <c r="K44" s="144" t="s">
+      <c r="G46" s="224"/>
+      <c r="H46" s="224"/>
+      <c r="I46" s="224"/>
+      <c r="J46" s="224"/>
+      <c r="K46" s="226" t="s">
         <v>59</v>
       </c>
-      <c r="L44" s="144"/>
-      <c r="M44" s="144"/>
-      <c r="N44" s="144"/>
-      <c r="O44" s="144"/>
-      <c r="P44" s="144"/>
-      <c r="Q44" s="144"/>
-      <c r="R44" s="146"/>
-    </row>
-    <row r="45" spans="2:20" s="20" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="133"/>
-      <c r="C45" s="143" t="s">
+      <c r="L46" s="226"/>
+      <c r="M46" s="226"/>
+      <c r="N46" s="226"/>
+      <c r="O46" s="226"/>
+      <c r="P46" s="226"/>
+      <c r="Q46" s="226"/>
+      <c r="R46" s="228"/>
+    </row>
+    <row r="47" spans="2:20" s="20" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="215"/>
+      <c r="C47" s="225" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="144"/>
-      <c r="E45" s="144"/>
-      <c r="F45" s="145" t="s">
+      <c r="D47" s="226"/>
+      <c r="E47" s="226"/>
+      <c r="F47" s="227" t="s">
         <v>58</v>
       </c>
-      <c r="G45" s="145"/>
-      <c r="H45" s="145"/>
-      <c r="I45" s="145"/>
-      <c r="J45" s="145"/>
-      <c r="K45" s="142" t="s">
+      <c r="G47" s="227"/>
+      <c r="H47" s="227"/>
+      <c r="I47" s="227"/>
+      <c r="J47" s="227"/>
+      <c r="K47" s="224" t="s">
         <v>60</v>
       </c>
-      <c r="L45" s="142"/>
-      <c r="M45" s="142"/>
-      <c r="N45" s="142"/>
-      <c r="O45" s="142"/>
-      <c r="P45" s="142"/>
-      <c r="Q45" s="142"/>
-      <c r="R45" s="147"/>
-    </row>
-    <row r="46" spans="2:20" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="133"/>
-      <c r="C46" s="99"/>
-      <c r="D46" s="80"/>
-      <c r="E46" s="80"/>
-      <c r="F46" s="80"/>
-      <c r="G46" s="80"/>
-      <c r="H46" s="80"/>
-      <c r="I46" s="80"/>
-      <c r="J46" s="80"/>
-      <c r="K46" s="80"/>
-      <c r="L46" s="80"/>
-      <c r="M46" s="80"/>
-      <c r="N46" s="80"/>
-      <c r="O46" s="97"/>
-      <c r="P46" s="81"/>
-      <c r="Q46" s="81"/>
-      <c r="R46" s="82"/>
-      <c r="S46" s="20"/>
-      <c r="T46" s="20"/>
-    </row>
-    <row r="47" spans="2:20" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="133"/>
-      <c r="C47" s="101"/>
-      <c r="D47" s="102" t="s">
+      <c r="L47" s="224"/>
+      <c r="M47" s="224"/>
+      <c r="N47" s="224"/>
+      <c r="O47" s="224"/>
+      <c r="P47" s="224"/>
+      <c r="Q47" s="224"/>
+      <c r="R47" s="229"/>
+    </row>
+    <row r="48" spans="2:20" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="215"/>
+      <c r="C48" s="99"/>
+      <c r="D48" s="80"/>
+      <c r="E48" s="80"/>
+      <c r="F48" s="80"/>
+      <c r="G48" s="80"/>
+      <c r="H48" s="80"/>
+      <c r="I48" s="80"/>
+      <c r="J48" s="80"/>
+      <c r="K48" s="80"/>
+      <c r="L48" s="80"/>
+      <c r="M48" s="80"/>
+      <c r="N48" s="80"/>
+      <c r="O48" s="97"/>
+      <c r="P48" s="81"/>
+      <c r="Q48" s="81"/>
+      <c r="R48" s="82"/>
+      <c r="S48" s="20"/>
+      <c r="T48" s="20"/>
+    </row>
+    <row r="49" spans="2:19" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="215"/>
+      <c r="C49" s="101"/>
+      <c r="D49" s="102" t="s">
         <v>81</v>
       </c>
-      <c r="E47" s="83"/>
-      <c r="F47" s="83"/>
-      <c r="G47" s="83"/>
-      <c r="H47" s="83"/>
-      <c r="I47" s="83"/>
-      <c r="J47" s="83"/>
-      <c r="K47" s="83"/>
-      <c r="L47" s="102" t="s">
+      <c r="E49" s="83"/>
+      <c r="F49" s="83"/>
+      <c r="G49" s="83"/>
+      <c r="H49" s="83"/>
+      <c r="I49" s="83"/>
+      <c r="J49" s="83"/>
+      <c r="K49" s="83"/>
+      <c r="L49" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="M47" s="76"/>
-      <c r="N47" s="83"/>
-      <c r="O47" s="96"/>
-      <c r="P47" s="84"/>
-      <c r="Q47" s="84"/>
-      <c r="R47" s="85"/>
-      <c r="S47" s="20"/>
-    </row>
-    <row r="48" spans="2:20" s="4" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="134"/>
-      <c r="C48" s="100"/>
-      <c r="D48" s="86"/>
-      <c r="E48" s="86"/>
-      <c r="F48" s="86"/>
-      <c r="G48" s="86"/>
-      <c r="H48" s="86"/>
-      <c r="I48" s="86"/>
-      <c r="J48" s="86"/>
-      <c r="K48" s="86"/>
-      <c r="L48" s="86"/>
-      <c r="M48" s="86"/>
-      <c r="N48" s="86"/>
-      <c r="O48" s="95"/>
-      <c r="P48" s="87"/>
-      <c r="Q48" s="87"/>
-      <c r="R48" s="88"/>
-      <c r="S48" s="20"/>
-    </row>
-    <row r="49" spans="2:19" s="4" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="215"/>
-      <c r="D49" s="216"/>
-      <c r="E49" s="216"/>
-      <c r="F49" s="216"/>
-      <c r="G49" s="216"/>
-      <c r="H49" s="216"/>
-      <c r="I49" s="216"/>
-      <c r="J49" s="216"/>
-      <c r="K49" s="216"/>
-      <c r="L49" s="216"/>
-      <c r="M49" s="216"/>
-      <c r="N49" s="216"/>
-      <c r="O49" s="216"/>
-      <c r="P49" s="216"/>
-      <c r="Q49" s="216"/>
-      <c r="R49" s="217"/>
+      <c r="M49" s="76"/>
+      <c r="N49" s="83"/>
+      <c r="O49" s="96"/>
+      <c r="P49" s="84"/>
+      <c r="Q49" s="84"/>
+      <c r="R49" s="85"/>
       <c r="S49" s="20"/>
     </row>
-    <row r="50" spans="2:19" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="26"/>
-      <c r="C50" s="195" t="s">
+    <row r="50" spans="2:19" s="4" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="216"/>
+      <c r="C50" s="100"/>
+      <c r="D50" s="86"/>
+      <c r="E50" s="86"/>
+      <c r="F50" s="86"/>
+      <c r="G50" s="86"/>
+      <c r="H50" s="86"/>
+      <c r="I50" s="86"/>
+      <c r="J50" s="86"/>
+      <c r="K50" s="86"/>
+      <c r="L50" s="86"/>
+      <c r="M50" s="86"/>
+      <c r="N50" s="86"/>
+      <c r="O50" s="95"/>
+      <c r="P50" s="87"/>
+      <c r="Q50" s="87"/>
+      <c r="R50" s="88"/>
+      <c r="S50" s="20"/>
+    </row>
+    <row r="51" spans="2:19" s="4" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="160"/>
+      <c r="D51" s="161"/>
+      <c r="E51" s="161"/>
+      <c r="F51" s="161"/>
+      <c r="G51" s="161"/>
+      <c r="H51" s="161"/>
+      <c r="I51" s="161"/>
+      <c r="J51" s="161"/>
+      <c r="K51" s="161"/>
+      <c r="L51" s="161"/>
+      <c r="M51" s="161"/>
+      <c r="N51" s="161"/>
+      <c r="O51" s="161"/>
+      <c r="P51" s="161"/>
+      <c r="Q51" s="161"/>
+      <c r="R51" s="162"/>
+      <c r="S51" s="20"/>
+    </row>
+    <row r="52" spans="2:19" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="26"/>
+      <c r="C52" s="140" t="s">
         <v>70</v>
       </c>
-      <c r="D50" s="196"/>
-      <c r="E50" s="196"/>
-      <c r="F50" s="196"/>
-      <c r="G50" s="197"/>
-      <c r="H50" s="201" t="s">
+      <c r="D52" s="141"/>
+      <c r="E52" s="141"/>
+      <c r="F52" s="141"/>
+      <c r="G52" s="142"/>
+      <c r="H52" s="146" t="s">
         <v>78</v>
       </c>
-      <c r="I50" s="196"/>
-      <c r="J50" s="196"/>
-      <c r="K50" s="196"/>
-      <c r="L50" s="197"/>
-      <c r="M50" s="203" t="s">
+      <c r="I52" s="141"/>
+      <c r="J52" s="141"/>
+      <c r="K52" s="141"/>
+      <c r="L52" s="142"/>
+      <c r="M52" s="148" t="s">
         <v>68</v>
       </c>
-      <c r="N50" s="204"/>
-      <c r="O50" s="205"/>
-      <c r="P50" s="203" t="s">
+      <c r="N52" s="149"/>
+      <c r="O52" s="150"/>
+      <c r="P52" s="148" t="s">
         <v>69</v>
       </c>
-      <c r="Q50" s="204"/>
-      <c r="R50" s="212"/>
-      <c r="S50" s="20"/>
-    </row>
-    <row r="51" spans="2:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="198"/>
-      <c r="D51" s="199"/>
-      <c r="E51" s="199"/>
-      <c r="F51" s="199"/>
-      <c r="G51" s="200"/>
-      <c r="H51" s="202"/>
-      <c r="I51" s="199"/>
-      <c r="J51" s="199"/>
-      <c r="K51" s="199"/>
-      <c r="L51" s="200"/>
-      <c r="M51" s="206"/>
-      <c r="N51" s="207"/>
-      <c r="O51" s="208"/>
-      <c r="P51" s="206"/>
-      <c r="Q51" s="207"/>
-      <c r="R51" s="213"/>
-      <c r="S51" s="20"/>
-    </row>
-    <row r="52" spans="2:19" s="5" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="52" t="s">
+      <c r="Q52" s="149"/>
+      <c r="R52" s="157"/>
+      <c r="S52" s="20"/>
+    </row>
+    <row r="53" spans="2:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C53" s="143"/>
+      <c r="D53" s="144"/>
+      <c r="E53" s="144"/>
+      <c r="F53" s="144"/>
+      <c r="G53" s="145"/>
+      <c r="H53" s="147"/>
+      <c r="I53" s="144"/>
+      <c r="J53" s="144"/>
+      <c r="K53" s="144"/>
+      <c r="L53" s="145"/>
+      <c r="M53" s="151"/>
+      <c r="N53" s="152"/>
+      <c r="O53" s="153"/>
+      <c r="P53" s="151"/>
+      <c r="Q53" s="152"/>
+      <c r="R53" s="158"/>
+      <c r="S53" s="20"/>
+    </row>
+    <row r="54" spans="2:19" s="5" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45"/>
-      <c r="F52" s="45"/>
-      <c r="G52" s="46"/>
-      <c r="H52" s="53" t="s">
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="45"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="I52" s="45"/>
-      <c r="J52" s="222"/>
-      <c r="K52" s="223"/>
-      <c r="L52" s="45"/>
-      <c r="M52" s="209"/>
-      <c r="N52" s="210"/>
-      <c r="O52" s="211"/>
-      <c r="P52" s="209"/>
-      <c r="Q52" s="210"/>
-      <c r="R52" s="214"/>
-      <c r="S52" s="24"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="167"/>
+      <c r="K54" s="168"/>
+      <c r="L54" s="45"/>
+      <c r="M54" s="154"/>
+      <c r="N54" s="155"/>
+      <c r="O54" s="156"/>
+      <c r="P54" s="154"/>
+      <c r="Q54" s="155"/>
+      <c r="R54" s="159"/>
+      <c r="S54" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="D25:O25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="F7:L7"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="D31:O31"/>
-    <mergeCell ref="D32:O32"/>
-    <mergeCell ref="D30:O30"/>
+    <mergeCell ref="B25:B38"/>
+    <mergeCell ref="E41:F43"/>
+    <mergeCell ref="G41:O41"/>
+    <mergeCell ref="C40:D43"/>
+    <mergeCell ref="B39:B50"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="C35:O35"/>
+    <mergeCell ref="C36:O36"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="F46:J46"/>
+    <mergeCell ref="F47:J47"/>
+    <mergeCell ref="K46:R46"/>
+    <mergeCell ref="K47:R47"/>
+    <mergeCell ref="D28:O28"/>
     <mergeCell ref="D29:O29"/>
-    <mergeCell ref="D28:O28"/>
-    <mergeCell ref="F14:L14"/>
-    <mergeCell ref="F8:R8"/>
-    <mergeCell ref="K43:R43"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="Q33:R34"/>
-    <mergeCell ref="C50:G51"/>
-    <mergeCell ref="H50:L51"/>
-    <mergeCell ref="M50:O52"/>
-    <mergeCell ref="P50:R52"/>
-    <mergeCell ref="C49:R49"/>
-    <mergeCell ref="P39:R41"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="J52:K52"/>
     <mergeCell ref="C4:H5"/>
     <mergeCell ref="I4:R5"/>
-    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q26:R26"/>
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="G18:N18"/>
     <mergeCell ref="O18:R18"/>
-    <mergeCell ref="D24:P24"/>
+    <mergeCell ref="D26:P26"/>
     <mergeCell ref="O20:Q20"/>
     <mergeCell ref="O21:Q21"/>
     <mergeCell ref="F9:R9"/>
@@ -3970,22 +4006,36 @@
     <mergeCell ref="N10:R10"/>
     <mergeCell ref="N12:R12"/>
     <mergeCell ref="F13:L13"/>
-    <mergeCell ref="B23:B36"/>
-    <mergeCell ref="E39:F41"/>
-    <mergeCell ref="G39:O39"/>
-    <mergeCell ref="C38:D41"/>
-    <mergeCell ref="B37:B48"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C33:O33"/>
-    <mergeCell ref="C34:O34"/>
-    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="K45:R45"/>
+    <mergeCell ref="P35:P36"/>
+    <mergeCell ref="Q35:R36"/>
+    <mergeCell ref="C52:G53"/>
+    <mergeCell ref="H52:L53"/>
+    <mergeCell ref="M52:O54"/>
+    <mergeCell ref="P52:R54"/>
+    <mergeCell ref="C51:R51"/>
+    <mergeCell ref="P41:R43"/>
     <mergeCell ref="C45:E45"/>
-    <mergeCell ref="F44:J44"/>
-    <mergeCell ref="F45:J45"/>
-    <mergeCell ref="K44:R44"/>
-    <mergeCell ref="K45:R45"/>
-    <mergeCell ref="D26:O26"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="F7:L7"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="D33:O33"/>
+    <mergeCell ref="D34:O34"/>
+    <mergeCell ref="D32:O32"/>
+    <mergeCell ref="D31:O31"/>
+    <mergeCell ref="D30:O30"/>
+    <mergeCell ref="F14:L14"/>
+    <mergeCell ref="F8:R8"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q34:R34"/>
     <mergeCell ref="D27:O27"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
ISP20221318 - Sample RFT Inspection 新增欄位
</commit_message>
<xml_diff>
--- a/Quality/Quality/XLT/InspBySPQuery_Detail.xlsx
+++ b/Quality/Quality/XLT/InspBySPQuery_Detail.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Inspection Report '!$B$1:$R$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Inspection Report '!$B$1:$R$55</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="90">
   <si>
     <t>TOTAL</t>
   </si>
@@ -721,6 +721,10 @@
   </si>
   <si>
     <t>Printing/AOP</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Badge</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
 </sst>
@@ -1880,252 +1884,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="9"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="9"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2208,6 +1966,252 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2232,13 +2236,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2246,7 +2250,7 @@
         <xdr:cNvPr id="4108" name="AutoShape 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C100000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C100000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2305,7 +2309,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2341,13 +2345,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>428609</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>11902</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>352409</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>142871</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2355,7 +2359,7 @@
         <xdr:cNvPr id="5" name="AutoShape 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2774,10 +2778,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T54"/>
+  <dimension ref="A1:T55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C4" sqref="C4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2801,42 +2805,42 @@
     <row r="1" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:20" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="169"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
-      <c r="H4" s="171"/>
-      <c r="I4" s="175" t="s">
+      <c r="C4" s="150"/>
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="151"/>
+      <c r="G4" s="151"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="176"/>
-      <c r="K4" s="176"/>
-      <c r="L4" s="176"/>
-      <c r="M4" s="176"/>
-      <c r="N4" s="176"/>
-      <c r="O4" s="176"/>
-      <c r="P4" s="176"/>
-      <c r="Q4" s="176"/>
-      <c r="R4" s="177"/>
+      <c r="J4" s="157"/>
+      <c r="K4" s="157"/>
+      <c r="L4" s="157"/>
+      <c r="M4" s="157"/>
+      <c r="N4" s="157"/>
+      <c r="O4" s="157"/>
+      <c r="P4" s="157"/>
+      <c r="Q4" s="157"/>
+      <c r="R4" s="158"/>
     </row>
     <row r="5" spans="1:20" ht="10.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="172"/>
-      <c r="D5" s="173"/>
-      <c r="E5" s="173"/>
-      <c r="F5" s="173"/>
-      <c r="G5" s="173"/>
-      <c r="H5" s="174"/>
-      <c r="I5" s="178"/>
-      <c r="J5" s="179"/>
-      <c r="K5" s="179"/>
-      <c r="L5" s="179"/>
-      <c r="M5" s="179"/>
-      <c r="N5" s="179"/>
-      <c r="O5" s="179"/>
-      <c r="P5" s="179"/>
-      <c r="Q5" s="179"/>
-      <c r="R5" s="180"/>
+      <c r="C5" s="153"/>
+      <c r="D5" s="154"/>
+      <c r="E5" s="154"/>
+      <c r="F5" s="154"/>
+      <c r="G5" s="154"/>
+      <c r="H5" s="155"/>
+      <c r="I5" s="159"/>
+      <c r="J5" s="160"/>
+      <c r="K5" s="160"/>
+      <c r="L5" s="160"/>
+      <c r="M5" s="160"/>
+      <c r="N5" s="160"/>
+      <c r="O5" s="160"/>
+      <c r="P5" s="160"/>
+      <c r="Q5" s="160"/>
+      <c r="R5" s="161"/>
     </row>
     <row r="6" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="7" t="s">
@@ -2852,11 +2856,11 @@
         <v>65</v>
       </c>
       <c r="I6" s="92"/>
-      <c r="J6" s="124" t="s">
+      <c r="J6" s="165" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="125"/>
-      <c r="L6" s="126"/>
+      <c r="K6" s="224"/>
+      <c r="L6" s="225"/>
       <c r="M6" s="29" t="s">
         <v>80</v>
       </c>
@@ -2875,13 +2879,13 @@
       <c r="E7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="123"/>
-      <c r="G7" s="122"/>
-      <c r="H7" s="122"/>
-      <c r="I7" s="122"/>
-      <c r="J7" s="122"/>
-      <c r="K7" s="122"/>
-      <c r="L7" s="122"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="149"/>
+      <c r="H7" s="149"/>
+      <c r="I7" s="149"/>
+      <c r="J7" s="149"/>
+      <c r="K7" s="149"/>
+      <c r="L7" s="149"/>
       <c r="M7" s="11"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -2900,19 +2904,19 @@
       <c r="E8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="129"/>
-      <c r="G8" s="130"/>
-      <c r="H8" s="130"/>
-      <c r="I8" s="130"/>
-      <c r="J8" s="130"/>
-      <c r="K8" s="130"/>
-      <c r="L8" s="130"/>
-      <c r="M8" s="130"/>
-      <c r="N8" s="130"/>
-      <c r="O8" s="130"/>
-      <c r="P8" s="130"/>
-      <c r="Q8" s="130"/>
-      <c r="R8" s="131"/>
+      <c r="F8" s="181"/>
+      <c r="G8" s="182"/>
+      <c r="H8" s="182"/>
+      <c r="I8" s="182"/>
+      <c r="J8" s="182"/>
+      <c r="K8" s="182"/>
+      <c r="L8" s="182"/>
+      <c r="M8" s="182"/>
+      <c r="N8" s="182"/>
+      <c r="O8" s="182"/>
+      <c r="P8" s="182"/>
+      <c r="Q8" s="182"/>
+      <c r="R8" s="183"/>
       <c r="S8" s="20"/>
     </row>
     <row r="9" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2925,19 +2929,19 @@
       <c r="E9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="129"/>
-      <c r="G9" s="130"/>
-      <c r="H9" s="130"/>
-      <c r="I9" s="130"/>
-      <c r="J9" s="130"/>
-      <c r="K9" s="130"/>
-      <c r="L9" s="130"/>
-      <c r="M9" s="130"/>
-      <c r="N9" s="130"/>
-      <c r="O9" s="130"/>
-      <c r="P9" s="130"/>
-      <c r="Q9" s="130"/>
-      <c r="R9" s="131"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="182"/>
+      <c r="H9" s="182"/>
+      <c r="I9" s="182"/>
+      <c r="J9" s="182"/>
+      <c r="K9" s="182"/>
+      <c r="L9" s="182"/>
+      <c r="M9" s="182"/>
+      <c r="N9" s="182"/>
+      <c r="O9" s="182"/>
+      <c r="P9" s="182"/>
+      <c r="Q9" s="182"/>
+      <c r="R9" s="183"/>
       <c r="S9" s="20"/>
     </row>
     <row r="10" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2948,21 +2952,21 @@
       <c r="E10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="123"/>
-      <c r="G10" s="122"/>
-      <c r="H10" s="122"/>
-      <c r="I10" s="122"/>
-      <c r="J10" s="122"/>
-      <c r="K10" s="122"/>
-      <c r="L10" s="122"/>
+      <c r="F10" s="184"/>
+      <c r="G10" s="149"/>
+      <c r="H10" s="149"/>
+      <c r="I10" s="149"/>
+      <c r="J10" s="149"/>
+      <c r="K10" s="149"/>
+      <c r="L10" s="149"/>
       <c r="M10" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="N10" s="123"/>
-      <c r="O10" s="199"/>
-      <c r="P10" s="199"/>
-      <c r="Q10" s="199"/>
-      <c r="R10" s="200"/>
+      <c r="N10" s="184"/>
+      <c r="O10" s="185"/>
+      <c r="P10" s="185"/>
+      <c r="Q10" s="185"/>
+      <c r="R10" s="186"/>
       <c r="S10" s="112"/>
       <c r="T10" s="116"/>
     </row>
@@ -2974,13 +2978,13 @@
       <c r="E11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="123"/>
-      <c r="G11" s="122"/>
-      <c r="H11" s="122"/>
-      <c r="I11" s="122"/>
-      <c r="J11" s="122"/>
-      <c r="K11" s="122"/>
-      <c r="L11" s="122"/>
+      <c r="F11" s="184"/>
+      <c r="G11" s="149"/>
+      <c r="H11" s="149"/>
+      <c r="I11" s="149"/>
+      <c r="J11" s="149"/>
+      <c r="K11" s="149"/>
+      <c r="L11" s="149"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -2997,21 +3001,21 @@
       <c r="E12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="123"/>
-      <c r="G12" s="122"/>
-      <c r="H12" s="122"/>
-      <c r="I12" s="122"/>
-      <c r="J12" s="122"/>
-      <c r="K12" s="122"/>
-      <c r="L12" s="122"/>
+      <c r="F12" s="184"/>
+      <c r="G12" s="149"/>
+      <c r="H12" s="149"/>
+      <c r="I12" s="149"/>
+      <c r="J12" s="149"/>
+      <c r="K12" s="149"/>
+      <c r="L12" s="149"/>
       <c r="M12" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="N12" s="123"/>
-      <c r="O12" s="199"/>
-      <c r="P12" s="199"/>
-      <c r="Q12" s="199"/>
-      <c r="R12" s="200"/>
+      <c r="N12" s="184"/>
+      <c r="O12" s="185"/>
+      <c r="P12" s="185"/>
+      <c r="Q12" s="185"/>
+      <c r="R12" s="186"/>
       <c r="S12" s="112"/>
       <c r="T12" s="112"/>
     </row>
@@ -3023,13 +3027,13 @@
       <c r="E13" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="123"/>
-      <c r="G13" s="122"/>
-      <c r="H13" s="122"/>
-      <c r="I13" s="122"/>
-      <c r="J13" s="122"/>
-      <c r="K13" s="122"/>
-      <c r="L13" s="122"/>
+      <c r="F13" s="184"/>
+      <c r="G13" s="149"/>
+      <c r="H13" s="149"/>
+      <c r="I13" s="149"/>
+      <c r="J13" s="149"/>
+      <c r="K13" s="149"/>
+      <c r="L13" s="149"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -3046,13 +3050,13 @@
       <c r="E14" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="F14" s="123"/>
-      <c r="G14" s="122"/>
-      <c r="H14" s="122"/>
-      <c r="I14" s="122"/>
-      <c r="J14" s="122"/>
-      <c r="K14" s="122"/>
-      <c r="L14" s="122"/>
+      <c r="F14" s="184"/>
+      <c r="G14" s="149"/>
+      <c r="H14" s="149"/>
+      <c r="I14" s="149"/>
+      <c r="J14" s="149"/>
+      <c r="K14" s="149"/>
+      <c r="L14" s="149"/>
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
       <c r="O14" s="25"/>
@@ -3139,28 +3143,28 @@
       <c r="S17" s="20"/>
     </row>
     <row r="18" spans="2:19" s="16" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="183" t="s">
+      <c r="C18" s="164" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="124"/>
-      <c r="E18" s="124"/>
-      <c r="F18" s="184"/>
-      <c r="G18" s="185" t="s">
+      <c r="D18" s="165"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="166"/>
+      <c r="G18" s="167" t="s">
         <v>77</v>
       </c>
-      <c r="H18" s="186"/>
-      <c r="I18" s="186"/>
-      <c r="J18" s="186"/>
-      <c r="K18" s="186"/>
-      <c r="L18" s="186"/>
-      <c r="M18" s="186"/>
-      <c r="N18" s="186"/>
-      <c r="O18" s="187" t="s">
+      <c r="H18" s="168"/>
+      <c r="I18" s="168"/>
+      <c r="J18" s="168"/>
+      <c r="K18" s="168"/>
+      <c r="L18" s="168"/>
+      <c r="M18" s="168"/>
+      <c r="N18" s="168"/>
+      <c r="O18" s="169" t="s">
         <v>13</v>
       </c>
-      <c r="P18" s="188"/>
-      <c r="Q18" s="188"/>
-      <c r="R18" s="189"/>
+      <c r="P18" s="170"/>
+      <c r="Q18" s="170"/>
+      <c r="R18" s="171"/>
       <c r="S18" s="22"/>
     </row>
     <row r="19" spans="2:19" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3211,11 +3215,11 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="94"/>
-      <c r="O20" s="193" t="s">
+      <c r="O20" s="175" t="s">
         <v>74</v>
       </c>
-      <c r="P20" s="194"/>
-      <c r="Q20" s="195"/>
+      <c r="P20" s="176"/>
+      <c r="Q20" s="177"/>
       <c r="R20" s="104"/>
       <c r="S20" s="20"/>
     </row>
@@ -3240,11 +3244,11 @@
         <v>73</v>
       </c>
       <c r="N21" s="94"/>
-      <c r="O21" s="196" t="s">
+      <c r="O21" s="178" t="s">
         <v>36</v>
       </c>
-      <c r="P21" s="197"/>
-      <c r="Q21" s="198"/>
+      <c r="P21" s="179"/>
+      <c r="Q21" s="180"/>
       <c r="R21" s="104"/>
       <c r="S21" s="103"/>
     </row>
@@ -3296,7 +3300,7 @@
       <c r="R23" s="104"/>
       <c r="S23" s="20"/>
     </row>
-    <row r="24" spans="2:19" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="48" t="s">
         <v>85</v>
       </c>
@@ -3317,686 +3321,721 @@
       <c r="R24" s="104"/>
       <c r="S24" s="20"/>
     </row>
-    <row r="25" spans="2:19" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="201" t="s">
+    <row r="25" spans="2:19" s="4" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="49"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="94"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="94"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="94"/>
+      <c r="O25" s="50"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="51"/>
+      <c r="R25" s="104"/>
+      <c r="S25" s="20"/>
+    </row>
+    <row r="26" spans="2:19" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C26" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="54"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="56"/>
-      <c r="P25" s="56"/>
-      <c r="Q25" s="56"/>
-      <c r="R25" s="105"/>
-    </row>
-    <row r="26" spans="2:19" s="23" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="202"/>
-      <c r="C26" s="57" t="s">
+      <c r="D26" s="54"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="56"/>
+      <c r="P26" s="56"/>
+      <c r="Q26" s="56"/>
+      <c r="R26" s="105"/>
+    </row>
+    <row r="27" spans="2:19" s="23" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="120"/>
+      <c r="C27" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="190" t="s">
+      <c r="D27" s="172" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="191"/>
-      <c r="F26" s="191"/>
-      <c r="G26" s="191"/>
-      <c r="H26" s="191"/>
-      <c r="I26" s="191"/>
-      <c r="J26" s="191"/>
-      <c r="K26" s="191"/>
-      <c r="L26" s="191"/>
-      <c r="M26" s="191"/>
-      <c r="N26" s="191"/>
-      <c r="O26" s="191"/>
-      <c r="P26" s="192"/>
-      <c r="Q26" s="181" t="s">
+      <c r="E27" s="173"/>
+      <c r="F27" s="173"/>
+      <c r="G27" s="173"/>
+      <c r="H27" s="173"/>
+      <c r="I27" s="173"/>
+      <c r="J27" s="173"/>
+      <c r="K27" s="173"/>
+      <c r="L27" s="173"/>
+      <c r="M27" s="173"/>
+      <c r="N27" s="173"/>
+      <c r="O27" s="173"/>
+      <c r="P27" s="174"/>
+      <c r="Q27" s="162" t="s">
         <v>14</v>
       </c>
-      <c r="R26" s="182"/>
-    </row>
-    <row r="27" spans="2:19" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="202"/>
-      <c r="C27" s="110"/>
-      <c r="D27" s="121"/>
-      <c r="E27" s="122"/>
-      <c r="F27" s="122"/>
-      <c r="G27" s="122"/>
-      <c r="H27" s="122"/>
-      <c r="I27" s="122"/>
-      <c r="J27" s="122"/>
-      <c r="K27" s="122"/>
-      <c r="L27" s="122"/>
-      <c r="M27" s="122"/>
-      <c r="N27" s="122"/>
-      <c r="O27" s="122"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="119"/>
-      <c r="R27" s="120"/>
+      <c r="R27" s="163"/>
     </row>
     <row r="28" spans="2:19" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="202"/>
+      <c r="B28" s="120"/>
       <c r="C28" s="110"/>
-      <c r="D28" s="121"/>
-      <c r="E28" s="122"/>
-      <c r="F28" s="122"/>
-      <c r="G28" s="122"/>
-      <c r="H28" s="122"/>
-      <c r="I28" s="122"/>
-      <c r="J28" s="122"/>
-      <c r="K28" s="122"/>
-      <c r="L28" s="122"/>
-      <c r="M28" s="122"/>
-      <c r="N28" s="122"/>
-      <c r="O28" s="122"/>
+      <c r="D28" s="148"/>
+      <c r="E28" s="149"/>
+      <c r="F28" s="149"/>
+      <c r="G28" s="149"/>
+      <c r="H28" s="149"/>
+      <c r="I28" s="149"/>
+      <c r="J28" s="149"/>
+      <c r="K28" s="149"/>
+      <c r="L28" s="149"/>
+      <c r="M28" s="149"/>
+      <c r="N28" s="149"/>
+      <c r="O28" s="149"/>
       <c r="P28" s="58"/>
-      <c r="Q28" s="119"/>
-      <c r="R28" s="120"/>
-    </row>
-    <row r="29" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="202"/>
-      <c r="C29" s="111"/>
-      <c r="D29" s="121"/>
-      <c r="E29" s="122"/>
-      <c r="F29" s="122"/>
-      <c r="G29" s="122"/>
-      <c r="H29" s="122"/>
-      <c r="I29" s="122"/>
-      <c r="J29" s="122"/>
-      <c r="K29" s="122"/>
-      <c r="L29" s="122"/>
-      <c r="M29" s="122"/>
-      <c r="N29" s="122"/>
-      <c r="O29" s="122"/>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="119"/>
-      <c r="R29" s="120"/>
+      <c r="Q28" s="228"/>
+      <c r="R28" s="229"/>
+    </row>
+    <row r="29" spans="2:19" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="120"/>
+      <c r="C29" s="110"/>
+      <c r="D29" s="148"/>
+      <c r="E29" s="149"/>
+      <c r="F29" s="149"/>
+      <c r="G29" s="149"/>
+      <c r="H29" s="149"/>
+      <c r="I29" s="149"/>
+      <c r="J29" s="149"/>
+      <c r="K29" s="149"/>
+      <c r="L29" s="149"/>
+      <c r="M29" s="149"/>
+      <c r="N29" s="149"/>
+      <c r="O29" s="149"/>
+      <c r="P29" s="58"/>
+      <c r="Q29" s="228"/>
+      <c r="R29" s="229"/>
     </row>
     <row r="30" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="202"/>
+      <c r="B30" s="120"/>
       <c r="C30" s="111"/>
-      <c r="D30" s="121"/>
-      <c r="E30" s="122"/>
-      <c r="F30" s="122"/>
-      <c r="G30" s="122"/>
-      <c r="H30" s="122"/>
-      <c r="I30" s="122"/>
-      <c r="J30" s="122"/>
-      <c r="K30" s="122"/>
-      <c r="L30" s="122"/>
-      <c r="M30" s="122"/>
-      <c r="N30" s="122"/>
-      <c r="O30" s="122"/>
+      <c r="D30" s="148"/>
+      <c r="E30" s="149"/>
+      <c r="F30" s="149"/>
+      <c r="G30" s="149"/>
+      <c r="H30" s="149"/>
+      <c r="I30" s="149"/>
+      <c r="J30" s="149"/>
+      <c r="K30" s="149"/>
+      <c r="L30" s="149"/>
+      <c r="M30" s="149"/>
+      <c r="N30" s="149"/>
+      <c r="O30" s="149"/>
       <c r="P30" s="59"/>
-      <c r="Q30" s="119"/>
-      <c r="R30" s="120"/>
+      <c r="Q30" s="228"/>
+      <c r="R30" s="229"/>
     </row>
     <row r="31" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="202"/>
+      <c r="B31" s="120"/>
       <c r="C31" s="111"/>
-      <c r="D31" s="121"/>
-      <c r="E31" s="122"/>
-      <c r="F31" s="122"/>
-      <c r="G31" s="122"/>
-      <c r="H31" s="122"/>
-      <c r="I31" s="122"/>
-      <c r="J31" s="122"/>
-      <c r="K31" s="122"/>
-      <c r="L31" s="122"/>
-      <c r="M31" s="122"/>
-      <c r="N31" s="122"/>
-      <c r="O31" s="122"/>
+      <c r="D31" s="148"/>
+      <c r="E31" s="149"/>
+      <c r="F31" s="149"/>
+      <c r="G31" s="149"/>
+      <c r="H31" s="149"/>
+      <c r="I31" s="149"/>
+      <c r="J31" s="149"/>
+      <c r="K31" s="149"/>
+      <c r="L31" s="149"/>
+      <c r="M31" s="149"/>
+      <c r="N31" s="149"/>
+      <c r="O31" s="149"/>
       <c r="P31" s="59"/>
-      <c r="Q31" s="119"/>
-      <c r="R31" s="120"/>
+      <c r="Q31" s="228"/>
+      <c r="R31" s="229"/>
     </row>
     <row r="32" spans="2:19" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="202"/>
+      <c r="B32" s="120"/>
       <c r="C32" s="111"/>
-      <c r="D32" s="121"/>
-      <c r="E32" s="122"/>
-      <c r="F32" s="122"/>
-      <c r="G32" s="122"/>
-      <c r="H32" s="122"/>
-      <c r="I32" s="122"/>
-      <c r="J32" s="122"/>
-      <c r="K32" s="122"/>
-      <c r="L32" s="122"/>
-      <c r="M32" s="122"/>
-      <c r="N32" s="122"/>
-      <c r="O32" s="122"/>
+      <c r="D32" s="148"/>
+      <c r="E32" s="149"/>
+      <c r="F32" s="149"/>
+      <c r="G32" s="149"/>
+      <c r="H32" s="149"/>
+      <c r="I32" s="149"/>
+      <c r="J32" s="149"/>
+      <c r="K32" s="149"/>
+      <c r="L32" s="149"/>
+      <c r="M32" s="149"/>
+      <c r="N32" s="149"/>
+      <c r="O32" s="149"/>
       <c r="P32" s="59"/>
-      <c r="Q32" s="119"/>
-      <c r="R32" s="120"/>
-    </row>
-    <row r="33" spans="2:20" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="202"/>
+      <c r="Q32" s="228"/>
+      <c r="R32" s="229"/>
+    </row>
+    <row r="33" spans="2:18" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="120"/>
       <c r="C33" s="111"/>
-      <c r="D33" s="121"/>
-      <c r="E33" s="122"/>
-      <c r="F33" s="122"/>
-      <c r="G33" s="122"/>
-      <c r="H33" s="122"/>
-      <c r="I33" s="122"/>
-      <c r="J33" s="122"/>
-      <c r="K33" s="122"/>
-      <c r="L33" s="122"/>
-      <c r="M33" s="122"/>
-      <c r="N33" s="122"/>
-      <c r="O33" s="122"/>
+      <c r="D33" s="148"/>
+      <c r="E33" s="149"/>
+      <c r="F33" s="149"/>
+      <c r="G33" s="149"/>
+      <c r="H33" s="149"/>
+      <c r="I33" s="149"/>
+      <c r="J33" s="149"/>
+      <c r="K33" s="149"/>
+      <c r="L33" s="149"/>
+      <c r="M33" s="149"/>
+      <c r="N33" s="149"/>
+      <c r="O33" s="149"/>
       <c r="P33" s="59"/>
-      <c r="Q33" s="119"/>
-      <c r="R33" s="120"/>
-    </row>
-    <row r="34" spans="2:20" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="202"/>
+      <c r="Q33" s="228"/>
+      <c r="R33" s="229"/>
+    </row>
+    <row r="34" spans="2:18" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="120"/>
       <c r="C34" s="111"/>
-      <c r="D34" s="121"/>
-      <c r="E34" s="122"/>
-      <c r="F34" s="122"/>
-      <c r="G34" s="122"/>
-      <c r="H34" s="122"/>
-      <c r="I34" s="122"/>
-      <c r="J34" s="122"/>
-      <c r="K34" s="122"/>
-      <c r="L34" s="122"/>
-      <c r="M34" s="122"/>
-      <c r="N34" s="122"/>
-      <c r="O34" s="122"/>
+      <c r="D34" s="148"/>
+      <c r="E34" s="149"/>
+      <c r="F34" s="149"/>
+      <c r="G34" s="149"/>
+      <c r="H34" s="149"/>
+      <c r="I34" s="149"/>
+      <c r="J34" s="149"/>
+      <c r="K34" s="149"/>
+      <c r="L34" s="149"/>
+      <c r="M34" s="149"/>
+      <c r="N34" s="149"/>
+      <c r="O34" s="149"/>
       <c r="P34" s="59"/>
-      <c r="Q34" s="119"/>
-      <c r="R34" s="120"/>
-    </row>
-    <row r="35" spans="2:20" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="202"/>
-      <c r="C35" s="217" t="s">
+      <c r="Q34" s="228"/>
+      <c r="R34" s="229"/>
+    </row>
+    <row r="35" spans="2:18" s="19" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="120"/>
+      <c r="C35" s="111"/>
+      <c r="D35" s="148"/>
+      <c r="E35" s="149"/>
+      <c r="F35" s="149"/>
+      <c r="G35" s="149"/>
+      <c r="H35" s="149"/>
+      <c r="I35" s="149"/>
+      <c r="J35" s="149"/>
+      <c r="K35" s="149"/>
+      <c r="L35" s="149"/>
+      <c r="M35" s="149"/>
+      <c r="N35" s="149"/>
+      <c r="O35" s="149"/>
+      <c r="P35" s="59"/>
+      <c r="Q35" s="228"/>
+      <c r="R35" s="229"/>
+    </row>
+    <row r="36" spans="2:18" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="120"/>
+      <c r="C36" s="135" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="218"/>
-      <c r="E35" s="218"/>
-      <c r="F35" s="218"/>
-      <c r="G35" s="218"/>
-      <c r="H35" s="218"/>
-      <c r="I35" s="218"/>
-      <c r="J35" s="218"/>
-      <c r="K35" s="218"/>
-      <c r="L35" s="218"/>
-      <c r="M35" s="218"/>
-      <c r="N35" s="218"/>
-      <c r="O35" s="219"/>
-      <c r="P35" s="134" t="s">
+      <c r="D36" s="136"/>
+      <c r="E36" s="136"/>
+      <c r="F36" s="136"/>
+      <c r="G36" s="136"/>
+      <c r="H36" s="136"/>
+      <c r="I36" s="136"/>
+      <c r="J36" s="136"/>
+      <c r="K36" s="136"/>
+      <c r="L36" s="136"/>
+      <c r="M36" s="136"/>
+      <c r="N36" s="136"/>
+      <c r="O36" s="137"/>
+      <c r="P36" s="189" t="s">
         <v>0</v>
       </c>
-      <c r="Q35" s="136"/>
-      <c r="R35" s="137"/>
-    </row>
-    <row r="36" spans="2:20" s="19" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="202"/>
-      <c r="C36" s="220" t="s">
+      <c r="Q36" s="191"/>
+      <c r="R36" s="192"/>
+    </row>
+    <row r="37" spans="2:18" s="19" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="120"/>
+      <c r="C37" s="138" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="221"/>
-      <c r="E36" s="221"/>
-      <c r="F36" s="221"/>
-      <c r="G36" s="221"/>
-      <c r="H36" s="221"/>
-      <c r="I36" s="221"/>
-      <c r="J36" s="221"/>
-      <c r="K36" s="221"/>
-      <c r="L36" s="221"/>
-      <c r="M36" s="221"/>
-      <c r="N36" s="221"/>
-      <c r="O36" s="222"/>
-      <c r="P36" s="135"/>
-      <c r="Q36" s="138"/>
-      <c r="R36" s="139"/>
-    </row>
-    <row r="37" spans="2:20" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="202"/>
-      <c r="C37" s="60" t="s">
+      <c r="D37" s="139"/>
+      <c r="E37" s="139"/>
+      <c r="F37" s="139"/>
+      <c r="G37" s="139"/>
+      <c r="H37" s="139"/>
+      <c r="I37" s="139"/>
+      <c r="J37" s="139"/>
+      <c r="K37" s="139"/>
+      <c r="L37" s="139"/>
+      <c r="M37" s="139"/>
+      <c r="N37" s="139"/>
+      <c r="O37" s="140"/>
+      <c r="P37" s="190"/>
+      <c r="Q37" s="193"/>
+      <c r="R37" s="194"/>
+    </row>
+    <row r="38" spans="2:18" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="120"/>
+      <c r="C38" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="61"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="93"/>
-      <c r="H37" s="93"/>
-      <c r="I37" s="61"/>
-      <c r="J37" s="61"/>
-      <c r="K37" s="61"/>
-      <c r="L37" s="106"/>
-      <c r="M37" s="61"/>
-      <c r="N37" s="61"/>
-      <c r="O37" s="61"/>
-      <c r="P37" s="61"/>
-      <c r="Q37" s="61"/>
-      <c r="R37" s="62"/>
-    </row>
-    <row r="38" spans="2:20" s="20" customFormat="1" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="202"/>
-      <c r="C38" s="98" t="s">
+      <c r="D38" s="61"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="61"/>
+      <c r="G38" s="93"/>
+      <c r="H38" s="93"/>
+      <c r="I38" s="61"/>
+      <c r="J38" s="61"/>
+      <c r="K38" s="61"/>
+      <c r="L38" s="106"/>
+      <c r="M38" s="61"/>
+      <c r="N38" s="61"/>
+      <c r="O38" s="61"/>
+      <c r="P38" s="61"/>
+      <c r="Q38" s="61"/>
+      <c r="R38" s="62"/>
+    </row>
+    <row r="39" spans="2:18" s="20" customFormat="1" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="120"/>
+      <c r="C39" s="98" t="s">
         <v>67</v>
       </c>
-      <c r="D38" s="66"/>
-      <c r="E38" s="66"/>
-      <c r="F38" s="66"/>
-      <c r="G38" s="66"/>
-      <c r="H38" s="66"/>
-      <c r="I38" s="66"/>
-      <c r="J38" s="66"/>
-      <c r="K38" s="66"/>
-      <c r="L38" s="66"/>
-      <c r="M38" s="66"/>
-      <c r="N38" s="66"/>
-      <c r="O38" s="66"/>
-      <c r="P38" s="66"/>
-      <c r="Q38" s="66"/>
-      <c r="R38" s="65"/>
-    </row>
-    <row r="39" spans="2:20" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="214" t="s">
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="66"/>
+      <c r="I39" s="66"/>
+      <c r="J39" s="66"/>
+      <c r="K39" s="66"/>
+      <c r="L39" s="66"/>
+      <c r="M39" s="66"/>
+      <c r="N39" s="66"/>
+      <c r="O39" s="66"/>
+      <c r="P39" s="66"/>
+      <c r="Q39" s="66"/>
+      <c r="R39" s="65"/>
+    </row>
+    <row r="40" spans="2:18" s="20" customFormat="1" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="132" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="209" t="s">
+      <c r="C40" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="210"/>
-      <c r="E39" s="210"/>
-      <c r="F39" s="211"/>
-      <c r="G39" s="127"/>
-      <c r="H39" s="128"/>
-      <c r="I39" s="67"/>
-      <c r="J39" s="67"/>
-      <c r="K39" s="67"/>
-      <c r="L39" s="67"/>
-      <c r="M39" s="67"/>
-      <c r="N39" s="67"/>
-      <c r="O39" s="67"/>
-      <c r="P39" s="67"/>
-      <c r="Q39" s="67"/>
-      <c r="R39" s="68"/>
-    </row>
-    <row r="40" spans="2:20" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="215"/>
-      <c r="C40" s="212"/>
-      <c r="D40" s="213"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="69"/>
-      <c r="G40" s="70"/>
-      <c r="H40" s="70"/>
-      <c r="I40" s="69"/>
-      <c r="J40" s="69"/>
-      <c r="K40" s="69"/>
-      <c r="L40" s="69"/>
-      <c r="M40" s="69"/>
-      <c r="N40" s="69"/>
-      <c r="O40" s="71"/>
-      <c r="P40" s="71"/>
-      <c r="Q40" s="71"/>
-      <c r="R40" s="72"/>
-    </row>
-    <row r="41" spans="2:20" s="20" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="215"/>
-      <c r="C41" s="212"/>
-      <c r="D41" s="213"/>
-      <c r="E41" s="203" t="s">
+      <c r="D40" s="128"/>
+      <c r="E40" s="128"/>
+      <c r="F40" s="129"/>
+      <c r="G40" s="226"/>
+      <c r="H40" s="227"/>
+      <c r="I40" s="67"/>
+      <c r="J40" s="67"/>
+      <c r="K40" s="67"/>
+      <c r="L40" s="67"/>
+      <c r="M40" s="67"/>
+      <c r="N40" s="67"/>
+      <c r="O40" s="67"/>
+      <c r="P40" s="67"/>
+      <c r="Q40" s="67"/>
+      <c r="R40" s="68"/>
+    </row>
+    <row r="41" spans="2:18" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="133"/>
+      <c r="C41" s="130"/>
+      <c r="D41" s="131"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="69"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="69"/>
+      <c r="J41" s="69"/>
+      <c r="K41" s="69"/>
+      <c r="L41" s="69"/>
+      <c r="M41" s="69"/>
+      <c r="N41" s="69"/>
+      <c r="O41" s="71"/>
+      <c r="P41" s="71"/>
+      <c r="Q41" s="71"/>
+      <c r="R41" s="72"/>
+    </row>
+    <row r="42" spans="2:18" s="20" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="133"/>
+      <c r="C42" s="130"/>
+      <c r="D42" s="131"/>
+      <c r="E42" s="121" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="204"/>
-      <c r="G41" s="209" t="s">
+      <c r="F42" s="122"/>
+      <c r="G42" s="127" t="s">
         <v>55</v>
       </c>
-      <c r="H41" s="210"/>
-      <c r="I41" s="210"/>
-      <c r="J41" s="210"/>
-      <c r="K41" s="210"/>
-      <c r="L41" s="210"/>
-      <c r="M41" s="210"/>
-      <c r="N41" s="210"/>
-      <c r="O41" s="211"/>
-      <c r="P41" s="163"/>
-      <c r="Q41" s="163"/>
-      <c r="R41" s="164"/>
-    </row>
-    <row r="42" spans="2:20" s="20" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="215"/>
-      <c r="C42" s="212"/>
-      <c r="D42" s="213"/>
-      <c r="E42" s="205"/>
-      <c r="F42" s="206"/>
-      <c r="G42" s="89" t="s">
+      <c r="H42" s="128"/>
+      <c r="I42" s="128"/>
+      <c r="J42" s="128"/>
+      <c r="K42" s="128"/>
+      <c r="L42" s="128"/>
+      <c r="M42" s="128"/>
+      <c r="N42" s="128"/>
+      <c r="O42" s="129"/>
+      <c r="P42" s="218"/>
+      <c r="Q42" s="218"/>
+      <c r="R42" s="219"/>
+    </row>
+    <row r="43" spans="2:18" s="20" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="133"/>
+      <c r="C43" s="130"/>
+      <c r="D43" s="131"/>
+      <c r="E43" s="123"/>
+      <c r="F43" s="124"/>
+      <c r="G43" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="H42" s="90" t="s">
+      <c r="H43" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="I42" s="90" t="s">
+      <c r="I43" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="J42" s="90" t="s">
+      <c r="J43" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="K42" s="90" t="s">
+      <c r="K43" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="L42" s="90" t="s">
+      <c r="L43" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="M42" s="90" t="s">
+      <c r="M43" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="N42" s="90" t="s">
+      <c r="N43" s="90" t="s">
         <v>49</v>
       </c>
-      <c r="O42" s="91" t="s">
+      <c r="O43" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="P42" s="163"/>
-      <c r="Q42" s="163"/>
-      <c r="R42" s="164"/>
-    </row>
-    <row r="43" spans="2:20" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="215"/>
-      <c r="C43" s="212"/>
-      <c r="D43" s="213"/>
-      <c r="E43" s="207"/>
-      <c r="F43" s="208"/>
-      <c r="G43" s="107"/>
-      <c r="H43" s="108"/>
-      <c r="I43" s="108"/>
-      <c r="J43" s="108"/>
-      <c r="K43" s="108"/>
-      <c r="L43" s="108"/>
-      <c r="M43" s="108"/>
-      <c r="N43" s="108"/>
-      <c r="O43" s="109"/>
-      <c r="P43" s="163"/>
-      <c r="Q43" s="163"/>
-      <c r="R43" s="164"/>
-    </row>
-    <row r="44" spans="2:20" s="20" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="215"/>
-      <c r="C44" s="73"/>
-      <c r="D44" s="74"/>
-      <c r="E44" s="75"/>
-      <c r="F44" s="75"/>
-      <c r="G44" s="76"/>
-      <c r="H44" s="76"/>
-      <c r="I44" s="76"/>
-      <c r="J44" s="76"/>
-      <c r="K44" s="76"/>
-      <c r="L44" s="76"/>
-      <c r="M44" s="76"/>
-      <c r="N44" s="76"/>
-      <c r="O44" s="76"/>
-      <c r="P44" s="77"/>
-      <c r="Q44" s="77"/>
-      <c r="R44" s="78"/>
-    </row>
-    <row r="45" spans="2:20" s="20" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="215"/>
-      <c r="C45" s="165" t="s">
+      <c r="P43" s="218"/>
+      <c r="Q43" s="218"/>
+      <c r="R43" s="219"/>
+    </row>
+    <row r="44" spans="2:18" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="133"/>
+      <c r="C44" s="130"/>
+      <c r="D44" s="131"/>
+      <c r="E44" s="125"/>
+      <c r="F44" s="126"/>
+      <c r="G44" s="107"/>
+      <c r="H44" s="108"/>
+      <c r="I44" s="108"/>
+      <c r="J44" s="108"/>
+      <c r="K44" s="108"/>
+      <c r="L44" s="108"/>
+      <c r="M44" s="108"/>
+      <c r="N44" s="108"/>
+      <c r="O44" s="109"/>
+      <c r="P44" s="218"/>
+      <c r="Q44" s="218"/>
+      <c r="R44" s="219"/>
+    </row>
+    <row r="45" spans="2:18" s="20" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="133"/>
+      <c r="C45" s="73"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="75"/>
+      <c r="F45" s="75"/>
+      <c r="G45" s="76"/>
+      <c r="H45" s="76"/>
+      <c r="I45" s="76"/>
+      <c r="J45" s="76"/>
+      <c r="K45" s="76"/>
+      <c r="L45" s="76"/>
+      <c r="M45" s="76"/>
+      <c r="N45" s="76"/>
+      <c r="O45" s="76"/>
+      <c r="P45" s="77"/>
+      <c r="Q45" s="77"/>
+      <c r="R45" s="78"/>
+    </row>
+    <row r="46" spans="2:18" s="20" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="133"/>
+      <c r="C46" s="220" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="166"/>
-      <c r="E45" s="166"/>
-      <c r="F45" s="79" t="s">
+      <c r="D46" s="221"/>
+      <c r="E46" s="221"/>
+      <c r="F46" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="G45" s="79"/>
-      <c r="H45" s="79"/>
-      <c r="I45" s="79"/>
-      <c r="J45" s="79"/>
-      <c r="K45" s="132" t="s">
+      <c r="G46" s="79"/>
+      <c r="H46" s="79"/>
+      <c r="I46" s="79"/>
+      <c r="J46" s="79"/>
+      <c r="K46" s="187" t="s">
         <v>63</v>
       </c>
-      <c r="L45" s="132"/>
-      <c r="M45" s="132"/>
-      <c r="N45" s="132"/>
-      <c r="O45" s="132"/>
-      <c r="P45" s="132"/>
-      <c r="Q45" s="132"/>
-      <c r="R45" s="133"/>
-    </row>
-    <row r="46" spans="2:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="215"/>
-      <c r="C46" s="223" t="s">
+      <c r="L46" s="187"/>
+      <c r="M46" s="187"/>
+      <c r="N46" s="187"/>
+      <c r="O46" s="187"/>
+      <c r="P46" s="187"/>
+      <c r="Q46" s="187"/>
+      <c r="R46" s="188"/>
+    </row>
+    <row r="47" spans="2:18" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="133"/>
+      <c r="C47" s="141" t="s">
         <v>61</v>
       </c>
-      <c r="D46" s="224"/>
-      <c r="E46" s="224"/>
-      <c r="F46" s="224" t="s">
+      <c r="D47" s="142"/>
+      <c r="E47" s="142"/>
+      <c r="F47" s="142" t="s">
         <v>62</v>
       </c>
-      <c r="G46" s="224"/>
-      <c r="H46" s="224"/>
-      <c r="I46" s="224"/>
-      <c r="J46" s="224"/>
-      <c r="K46" s="226" t="s">
+      <c r="G47" s="142"/>
+      <c r="H47" s="142"/>
+      <c r="I47" s="142"/>
+      <c r="J47" s="142"/>
+      <c r="K47" s="144" t="s">
         <v>59</v>
       </c>
-      <c r="L46" s="226"/>
-      <c r="M46" s="226"/>
-      <c r="N46" s="226"/>
-      <c r="O46" s="226"/>
-      <c r="P46" s="226"/>
-      <c r="Q46" s="226"/>
-      <c r="R46" s="228"/>
-    </row>
-    <row r="47" spans="2:20" s="20" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="215"/>
-      <c r="C47" s="225" t="s">
+      <c r="L47" s="144"/>
+      <c r="M47" s="144"/>
+      <c r="N47" s="144"/>
+      <c r="O47" s="144"/>
+      <c r="P47" s="144"/>
+      <c r="Q47" s="144"/>
+      <c r="R47" s="146"/>
+    </row>
+    <row r="48" spans="2:18" s="20" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="133"/>
+      <c r="C48" s="143" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="226"/>
-      <c r="E47" s="226"/>
-      <c r="F47" s="227" t="s">
+      <c r="D48" s="144"/>
+      <c r="E48" s="144"/>
+      <c r="F48" s="145" t="s">
         <v>58</v>
       </c>
-      <c r="G47" s="227"/>
-      <c r="H47" s="227"/>
-      <c r="I47" s="227"/>
-      <c r="J47" s="227"/>
-      <c r="K47" s="224" t="s">
+      <c r="G48" s="145"/>
+      <c r="H48" s="145"/>
+      <c r="I48" s="145"/>
+      <c r="J48" s="145"/>
+      <c r="K48" s="142" t="s">
         <v>60</v>
       </c>
-      <c r="L47" s="224"/>
-      <c r="M47" s="224"/>
-      <c r="N47" s="224"/>
-      <c r="O47" s="224"/>
-      <c r="P47" s="224"/>
-      <c r="Q47" s="224"/>
-      <c r="R47" s="229"/>
-    </row>
-    <row r="48" spans="2:20" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="215"/>
-      <c r="C48" s="99"/>
-      <c r="D48" s="80"/>
-      <c r="E48" s="80"/>
-      <c r="F48" s="80"/>
-      <c r="G48" s="80"/>
-      <c r="H48" s="80"/>
-      <c r="I48" s="80"/>
-      <c r="J48" s="80"/>
-      <c r="K48" s="80"/>
-      <c r="L48" s="80"/>
-      <c r="M48" s="80"/>
-      <c r="N48" s="80"/>
-      <c r="O48" s="97"/>
-      <c r="P48" s="81"/>
-      <c r="Q48" s="81"/>
-      <c r="R48" s="82"/>
-      <c r="S48" s="20"/>
-      <c r="T48" s="20"/>
-    </row>
-    <row r="49" spans="2:19" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="215"/>
-      <c r="C49" s="101"/>
-      <c r="D49" s="102" t="s">
+      <c r="L48" s="142"/>
+      <c r="M48" s="142"/>
+      <c r="N48" s="142"/>
+      <c r="O48" s="142"/>
+      <c r="P48" s="142"/>
+      <c r="Q48" s="142"/>
+      <c r="R48" s="147"/>
+    </row>
+    <row r="49" spans="2:20" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="133"/>
+      <c r="C49" s="99"/>
+      <c r="D49" s="80"/>
+      <c r="E49" s="80"/>
+      <c r="F49" s="80"/>
+      <c r="G49" s="80"/>
+      <c r="H49" s="80"/>
+      <c r="I49" s="80"/>
+      <c r="J49" s="80"/>
+      <c r="K49" s="80"/>
+      <c r="L49" s="80"/>
+      <c r="M49" s="80"/>
+      <c r="N49" s="80"/>
+      <c r="O49" s="97"/>
+      <c r="P49" s="81"/>
+      <c r="Q49" s="81"/>
+      <c r="R49" s="82"/>
+      <c r="S49" s="20"/>
+      <c r="T49" s="20"/>
+    </row>
+    <row r="50" spans="2:20" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="133"/>
+      <c r="C50" s="101"/>
+      <c r="D50" s="102" t="s">
         <v>81</v>
       </c>
-      <c r="E49" s="83"/>
-      <c r="F49" s="83"/>
-      <c r="G49" s="83"/>
-      <c r="H49" s="83"/>
-      <c r="I49" s="83"/>
-      <c r="J49" s="83"/>
-      <c r="K49" s="83"/>
-      <c r="L49" s="102" t="s">
+      <c r="E50" s="83"/>
+      <c r="F50" s="83"/>
+      <c r="G50" s="83"/>
+      <c r="H50" s="83"/>
+      <c r="I50" s="83"/>
+      <c r="J50" s="83"/>
+      <c r="K50" s="83"/>
+      <c r="L50" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="M49" s="76"/>
-      <c r="N49" s="83"/>
-      <c r="O49" s="96"/>
-      <c r="P49" s="84"/>
-      <c r="Q49" s="84"/>
-      <c r="R49" s="85"/>
-      <c r="S49" s="20"/>
-    </row>
-    <row r="50" spans="2:19" s="4" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="216"/>
-      <c r="C50" s="100"/>
-      <c r="D50" s="86"/>
-      <c r="E50" s="86"/>
-      <c r="F50" s="86"/>
-      <c r="G50" s="86"/>
-      <c r="H50" s="86"/>
-      <c r="I50" s="86"/>
-      <c r="J50" s="86"/>
-      <c r="K50" s="86"/>
-      <c r="L50" s="86"/>
-      <c r="M50" s="86"/>
-      <c r="N50" s="86"/>
-      <c r="O50" s="95"/>
-      <c r="P50" s="87"/>
-      <c r="Q50" s="87"/>
-      <c r="R50" s="88"/>
+      <c r="M50" s="76"/>
+      <c r="N50" s="83"/>
+      <c r="O50" s="96"/>
+      <c r="P50" s="84"/>
+      <c r="Q50" s="84"/>
+      <c r="R50" s="85"/>
       <c r="S50" s="20"/>
     </row>
-    <row r="51" spans="2:19" s="4" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="160"/>
-      <c r="D51" s="161"/>
-      <c r="E51" s="161"/>
-      <c r="F51" s="161"/>
-      <c r="G51" s="161"/>
-      <c r="H51" s="161"/>
-      <c r="I51" s="161"/>
-      <c r="J51" s="161"/>
-      <c r="K51" s="161"/>
-      <c r="L51" s="161"/>
-      <c r="M51" s="161"/>
-      <c r="N51" s="161"/>
-      <c r="O51" s="161"/>
-      <c r="P51" s="161"/>
-      <c r="Q51" s="161"/>
-      <c r="R51" s="162"/>
+    <row r="51" spans="2:20" s="4" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="134"/>
+      <c r="C51" s="100"/>
+      <c r="D51" s="86"/>
+      <c r="E51" s="86"/>
+      <c r="F51" s="86"/>
+      <c r="G51" s="86"/>
+      <c r="H51" s="86"/>
+      <c r="I51" s="86"/>
+      <c r="J51" s="86"/>
+      <c r="K51" s="86"/>
+      <c r="L51" s="86"/>
+      <c r="M51" s="86"/>
+      <c r="N51" s="86"/>
+      <c r="O51" s="95"/>
+      <c r="P51" s="87"/>
+      <c r="Q51" s="87"/>
+      <c r="R51" s="88"/>
       <c r="S51" s="20"/>
     </row>
-    <row r="52" spans="2:19" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="26"/>
-      <c r="C52" s="140" t="s">
+    <row r="52" spans="2:20" s="4" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="215"/>
+      <c r="D52" s="216"/>
+      <c r="E52" s="216"/>
+      <c r="F52" s="216"/>
+      <c r="G52" s="216"/>
+      <c r="H52" s="216"/>
+      <c r="I52" s="216"/>
+      <c r="J52" s="216"/>
+      <c r="K52" s="216"/>
+      <c r="L52" s="216"/>
+      <c r="M52" s="216"/>
+      <c r="N52" s="216"/>
+      <c r="O52" s="216"/>
+      <c r="P52" s="216"/>
+      <c r="Q52" s="216"/>
+      <c r="R52" s="217"/>
+      <c r="S52" s="20"/>
+    </row>
+    <row r="53" spans="2:20" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="26"/>
+      <c r="C53" s="195" t="s">
         <v>70</v>
       </c>
-      <c r="D52" s="141"/>
-      <c r="E52" s="141"/>
-      <c r="F52" s="141"/>
-      <c r="G52" s="142"/>
-      <c r="H52" s="146" t="s">
+      <c r="D53" s="196"/>
+      <c r="E53" s="196"/>
+      <c r="F53" s="196"/>
+      <c r="G53" s="197"/>
+      <c r="H53" s="201" t="s">
         <v>78</v>
       </c>
-      <c r="I52" s="141"/>
-      <c r="J52" s="141"/>
-      <c r="K52" s="141"/>
-      <c r="L52" s="142"/>
-      <c r="M52" s="148" t="s">
+      <c r="I53" s="196"/>
+      <c r="J53" s="196"/>
+      <c r="K53" s="196"/>
+      <c r="L53" s="197"/>
+      <c r="M53" s="203" t="s">
         <v>68</v>
       </c>
-      <c r="N52" s="149"/>
-      <c r="O52" s="150"/>
-      <c r="P52" s="148" t="s">
+      <c r="N53" s="204"/>
+      <c r="O53" s="205"/>
+      <c r="P53" s="203" t="s">
         <v>69</v>
       </c>
-      <c r="Q52" s="149"/>
-      <c r="R52" s="157"/>
-      <c r="S52" s="20"/>
-    </row>
-    <row r="53" spans="2:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C53" s="143"/>
-      <c r="D53" s="144"/>
-      <c r="E53" s="144"/>
-      <c r="F53" s="144"/>
-      <c r="G53" s="145"/>
-      <c r="H53" s="147"/>
-      <c r="I53" s="144"/>
-      <c r="J53" s="144"/>
-      <c r="K53" s="144"/>
-      <c r="L53" s="145"/>
-      <c r="M53" s="151"/>
-      <c r="N53" s="152"/>
-      <c r="O53" s="153"/>
-      <c r="P53" s="151"/>
-      <c r="Q53" s="152"/>
-      <c r="R53" s="158"/>
+      <c r="Q53" s="204"/>
+      <c r="R53" s="212"/>
       <c r="S53" s="20"/>
     </row>
-    <row r="54" spans="2:19" s="5" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="52" t="s">
+    <row r="54" spans="2:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="198"/>
+      <c r="D54" s="199"/>
+      <c r="E54" s="199"/>
+      <c r="F54" s="199"/>
+      <c r="G54" s="200"/>
+      <c r="H54" s="202"/>
+      <c r="I54" s="199"/>
+      <c r="J54" s="199"/>
+      <c r="K54" s="199"/>
+      <c r="L54" s="200"/>
+      <c r="M54" s="206"/>
+      <c r="N54" s="207"/>
+      <c r="O54" s="208"/>
+      <c r="P54" s="206"/>
+      <c r="Q54" s="207"/>
+      <c r="R54" s="213"/>
+      <c r="S54" s="20"/>
+    </row>
+    <row r="55" spans="2:20" s="5" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D54" s="45"/>
-      <c r="E54" s="45"/>
-      <c r="F54" s="45"/>
-      <c r="G54" s="46"/>
-      <c r="H54" s="53" t="s">
+      <c r="D55" s="45"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="I54" s="45"/>
-      <c r="J54" s="167"/>
-      <c r="K54" s="168"/>
-      <c r="L54" s="45"/>
-      <c r="M54" s="154"/>
-      <c r="N54" s="155"/>
-      <c r="O54" s="156"/>
-      <c r="P54" s="154"/>
-      <c r="Q54" s="155"/>
-      <c r="R54" s="159"/>
-      <c r="S54" s="24"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="222"/>
+      <c r="K55" s="223"/>
+      <c r="L55" s="45"/>
+      <c r="M55" s="209"/>
+      <c r="N55" s="210"/>
+      <c r="O55" s="211"/>
+      <c r="P55" s="209"/>
+      <c r="Q55" s="210"/>
+      <c r="R55" s="214"/>
+      <c r="S55" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="B25:B38"/>
-    <mergeCell ref="E41:F43"/>
-    <mergeCell ref="G41:O41"/>
-    <mergeCell ref="C40:D43"/>
-    <mergeCell ref="B39:B50"/>
-    <mergeCell ref="C39:F39"/>
-    <mergeCell ref="C35:O35"/>
-    <mergeCell ref="C36:O36"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="F7:L7"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="D34:O34"/>
+    <mergeCell ref="D35:O35"/>
+    <mergeCell ref="D33:O33"/>
+    <mergeCell ref="D32:O32"/>
+    <mergeCell ref="D31:O31"/>
+    <mergeCell ref="F14:L14"/>
+    <mergeCell ref="F8:R8"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="D28:O28"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="K46:R46"/>
+    <mergeCell ref="P36:P37"/>
+    <mergeCell ref="Q36:R37"/>
+    <mergeCell ref="C53:G54"/>
+    <mergeCell ref="H53:L54"/>
+    <mergeCell ref="M53:O55"/>
+    <mergeCell ref="P53:R55"/>
+    <mergeCell ref="C52:R52"/>
+    <mergeCell ref="P42:R44"/>
     <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="F46:J46"/>
-    <mergeCell ref="F47:J47"/>
-    <mergeCell ref="K46:R46"/>
-    <mergeCell ref="K47:R47"/>
-    <mergeCell ref="D28:O28"/>
-    <mergeCell ref="D29:O29"/>
+    <mergeCell ref="J55:K55"/>
     <mergeCell ref="C4:H5"/>
     <mergeCell ref="I4:R5"/>
-    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="G18:N18"/>
     <mergeCell ref="O18:R18"/>
-    <mergeCell ref="D26:P26"/>
+    <mergeCell ref="D27:P27"/>
     <mergeCell ref="O20:Q20"/>
     <mergeCell ref="O21:Q21"/>
     <mergeCell ref="F9:R9"/>
@@ -4006,36 +4045,22 @@
     <mergeCell ref="N10:R10"/>
     <mergeCell ref="N12:R12"/>
     <mergeCell ref="F13:L13"/>
-    <mergeCell ref="K45:R45"/>
-    <mergeCell ref="P35:P36"/>
-    <mergeCell ref="Q35:R36"/>
-    <mergeCell ref="C52:G53"/>
-    <mergeCell ref="H52:L53"/>
-    <mergeCell ref="M52:O54"/>
-    <mergeCell ref="P52:R54"/>
-    <mergeCell ref="C51:R51"/>
-    <mergeCell ref="P41:R43"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="F7:L7"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="D33:O33"/>
-    <mergeCell ref="D34:O34"/>
-    <mergeCell ref="D32:O32"/>
-    <mergeCell ref="D31:O31"/>
+    <mergeCell ref="B26:B39"/>
+    <mergeCell ref="E42:F44"/>
+    <mergeCell ref="G42:O42"/>
+    <mergeCell ref="C41:D44"/>
+    <mergeCell ref="B40:B51"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C36:O36"/>
+    <mergeCell ref="C37:O37"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="F47:J47"/>
+    <mergeCell ref="F48:J48"/>
+    <mergeCell ref="K47:R47"/>
+    <mergeCell ref="K48:R48"/>
+    <mergeCell ref="D29:O29"/>
     <mergeCell ref="D30:O30"/>
-    <mergeCell ref="F14:L14"/>
-    <mergeCell ref="F8:R8"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="D27:O27"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>